<commit_message>
Add spring break road trip history
</commit_message>
<xml_diff>
--- a/english.xlsx
+++ b/english.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popoves\Desktop\experience\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BBD052-4561-4A7E-A239-FA1E3E6057F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBACB894-F367-4217-BFA7-5F38AAD36FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AF848DA1-86EF-4FED-9942-D008ADCF70E9}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="757">
   <si>
     <t>word</t>
   </si>
@@ -1715,9 +1715,6 @@
     <t>we considered flying, but it is too expensive to fly with three kids</t>
   </si>
   <si>
-    <t>мы думали полететь, но лететь с тремя детьми очень дорого</t>
-  </si>
-  <si>
     <t>particularly expensive</t>
   </si>
   <si>
@@ -1745,24 +1742,12 @@
     <t>кроме того</t>
   </si>
   <si>
-    <t>when we get to our destination</t>
-  </si>
-  <si>
-    <t>когда мы доберемся до местоназначения</t>
-  </si>
-  <si>
     <t>we would have</t>
   </si>
   <si>
     <t>нам придется</t>
   </si>
   <si>
-    <t>to rent car</t>
-  </si>
-  <si>
-    <t>арендовать машину</t>
-  </si>
-  <si>
     <t>besides, when we get to our destination, we would have to rent a car</t>
   </si>
   <si>
@@ -1790,18 +1775,6 @@
     <t>дешево</t>
   </si>
   <si>
-    <t>driving</t>
-  </si>
-  <si>
-    <t>поездка на машине</t>
-  </si>
-  <si>
-    <t>much better option</t>
-  </si>
-  <si>
-    <t>гораздо лучший вариант</t>
-  </si>
-  <si>
     <t>driving is a much better option</t>
   </si>
   <si>
@@ -1826,15 +1799,9 @@
     <t>мы можем остановиться</t>
   </si>
   <si>
-    <t>visit places on the way</t>
-  </si>
-  <si>
     <t>посещать мета по пути</t>
   </si>
   <si>
-    <t>it takes more time and it is more tiring, but we can stop and visit places on the way</t>
-  </si>
-  <si>
     <t>это займет больше времени и это более утомительно, но мы можем остановиться и посетить мета по пути</t>
   </si>
   <si>
@@ -1850,15 +1817,9 @@
     <t>он имеет достаточно места для нас</t>
   </si>
   <si>
-    <t>out luggage</t>
-  </si>
-  <si>
     <t>наш багаж</t>
   </si>
   <si>
-    <t>we have mini-van that has enough space for us and out luggage</t>
-  </si>
-  <si>
     <t>у нас есть мини-вен, в котором достаточно места для нас и нашего багажа</t>
   </si>
   <si>
@@ -1949,247 +1910,394 @@
     <t>симпатичный</t>
   </si>
   <si>
-    <t>spring breaks</t>
-  </si>
-  <si>
     <t>there are many places</t>
   </si>
   <si>
     <t>seven wonders of the world</t>
   </si>
   <si>
-    <t>spring break is a a great time to go on vacation</t>
-  </si>
-  <si>
     <t>there are many places we want to visit</t>
   </si>
   <si>
+    <t>it will take us two days</t>
+  </si>
+  <si>
+    <t>это займет у нас 2 дня</t>
+  </si>
+  <si>
+    <t>to get to our destination</t>
+  </si>
+  <si>
+    <t>добираться до метса назначения</t>
+  </si>
+  <si>
+    <t>it will take us two days to get to our destination</t>
+  </si>
+  <si>
+    <t>нам понадобится два дня, чтобы добраться до места назначения</t>
+  </si>
+  <si>
+    <t>we also booked a hotel</t>
+  </si>
+  <si>
+    <t>мы так же забронировали отель</t>
+  </si>
+  <si>
+    <t>where we can stay</t>
+  </si>
+  <si>
+    <t>где мы можем остановиться</t>
+  </si>
+  <si>
+    <t>на ночь</t>
+  </si>
+  <si>
+    <t>for the night</t>
+  </si>
+  <si>
+    <t>we also booked a hotel where we can stay for the night</t>
+  </si>
+  <si>
+    <t>мы так же забронировали отель, где мы можем остановиться на ночь</t>
+  </si>
+  <si>
+    <t>the hotel provides breakfast</t>
+  </si>
+  <si>
+    <t>отель предоставляет завтрак</t>
+  </si>
+  <si>
+    <t>нам не нужно беспокоиться о</t>
+  </si>
+  <si>
+    <t>finding food in the morning</t>
+  </si>
+  <si>
+    <t>поиск еды на утро</t>
+  </si>
+  <si>
+    <t>we don’t need to worry about finding food in the morning</t>
+  </si>
+  <si>
+    <t>нам не унжно беспокоиться о поиске еды на утро</t>
+  </si>
+  <si>
+    <t>it is very convinient</t>
+  </si>
+  <si>
+    <t>это очень удобно</t>
+  </si>
+  <si>
+    <t>and usually</t>
+  </si>
+  <si>
+    <t>и обычно</t>
+  </si>
+  <si>
+    <t>food is quite good</t>
+  </si>
+  <si>
+    <t>еда довольно вкусная</t>
+  </si>
+  <si>
+    <t>it is very convinient, and usually, the food is quite good</t>
+  </si>
+  <si>
+    <t>we can quickly eat</t>
+  </si>
+  <si>
+    <t>мы можем быстро поесть</t>
+  </si>
+  <si>
+    <t>check out</t>
+  </si>
+  <si>
+    <t>выписаться из отеля</t>
+  </si>
+  <si>
+    <t>and continue our journey</t>
+  </si>
+  <si>
+    <t>и продолжить наше путешествие</t>
+  </si>
+  <si>
+    <t>we can quickly eat, check out, and continue our journey</t>
+  </si>
+  <si>
+    <t>мы можем быстро поесть, выписаться из отеля и продолжить наше путишествие</t>
+  </si>
+  <si>
+    <t>we always plan</t>
+  </si>
+  <si>
+    <t>мы всегда планируем</t>
+  </si>
+  <si>
+    <t>we always plan on leaving early in the morning, so we have plenty of time to drive</t>
+  </si>
+  <si>
+    <t>мы всегда планируем отъезд рано утром, так, чтобы иметь достаточно времени на дорогу</t>
+  </si>
+  <si>
+    <t>but when you have children</t>
+  </si>
+  <si>
+    <t>но когда у вас есть дети</t>
+  </si>
+  <si>
+    <t>it is very difficult to leave early</t>
+  </si>
+  <si>
+    <t>это очень сложно  - выезжать рано</t>
+  </si>
+  <si>
+    <t>but when your have children, it is very difficult to leave early</t>
+  </si>
+  <si>
+    <t>но когда у вас есть дети, то сложно выезжать рано</t>
+  </si>
+  <si>
+    <t>I just hope</t>
+  </si>
+  <si>
+    <t>я просто надеюсь</t>
+  </si>
+  <si>
+    <t>we get to hotel</t>
+  </si>
+  <si>
+    <t>мы добераемся до отеля</t>
+  </si>
+  <si>
+    <t>I just hope we get to hotel before it gets dark</t>
+  </si>
+  <si>
+    <t>it is hard to me</t>
+  </si>
+  <si>
+    <t>to drive at night</t>
+  </si>
+  <si>
+    <t>ехать ночью</t>
+  </si>
+  <si>
+    <t>it is hard to me to drive at night</t>
+  </si>
+  <si>
+    <t>это сложно для меня - ехать ночью</t>
+  </si>
+  <si>
+    <t>вам нравится путешествовать?</t>
+  </si>
+  <si>
+    <t>do you like traveling?</t>
+  </si>
+  <si>
+    <t>do you have any plans for the spring break?</t>
+  </si>
+  <si>
+    <t>let me know in the comments</t>
+  </si>
+  <si>
+    <t>дайте мне знать об этом в коментариях</t>
+  </si>
+  <si>
+    <t>try your best to practice</t>
+  </si>
+  <si>
+    <t>старайтесь изо всех сил практиковаться</t>
+  </si>
+  <si>
+    <t>write your comments in English</t>
+  </si>
+  <si>
+    <t>пишите ваши комментарии на английском</t>
+  </si>
+  <si>
+    <t>try your best to practice and write your comments in English</t>
+  </si>
+  <si>
+    <t>старайтесь изо всех сил и  пишите ваши коментарии на английском</t>
+  </si>
+  <si>
+    <t>don’t worry about mistakes</t>
+  </si>
+  <si>
+    <t>не волнуйтесь об ошибках</t>
+  </si>
+  <si>
+    <t>I will be happy</t>
+  </si>
+  <si>
+    <t>я буду счастлив</t>
+  </si>
+  <si>
+    <t>to correct them for you</t>
+  </si>
+  <si>
+    <t>исправить их для вас</t>
+  </si>
+  <si>
+    <t>I will be happy to correct them for you</t>
+  </si>
+  <si>
+    <t>я буду рад исправить их для вас</t>
+  </si>
+  <si>
+    <t>to visit places on the way</t>
+  </si>
+  <si>
+    <t>мы рассматривали вариант полета на самолете, но лететь с тремя детьми очень дорого</t>
+  </si>
+  <si>
+    <t>it takes more time and it is more tiring, but we can to stop and visit places on the way</t>
+  </si>
+  <si>
+    <t>our luggage</t>
+  </si>
+  <si>
+    <t>we have mini-van that has enough space for us and our luggage</t>
+  </si>
+  <si>
+    <t>we don’t need to worry about</t>
+  </si>
+  <si>
+    <t>это очень удобно, и обычно эта еда довольно хорошая</t>
+  </si>
+  <si>
+    <t>у нас есть достаточно времени</t>
+  </si>
+  <si>
+    <t>у нас есть достаточно времени на дорогу</t>
+  </si>
+  <si>
+    <t>мы всегда планируем отъезд рано утром</t>
+  </si>
+  <si>
+    <t>we alwase plan on leaving early in the morning</t>
+  </si>
+  <si>
+    <t>we have plenty of time</t>
+  </si>
+  <si>
+    <t>we have plenty of time to drive</t>
+  </si>
+  <si>
+    <t>я надеюсь что мы доберемся до отеля до того как стемнеет</t>
+  </si>
+  <si>
+    <t>мы доберемся до отеля до того как стемнеет</t>
+  </si>
+  <si>
+    <t>we get to hotel before it gets dark</t>
+  </si>
+  <si>
+    <t>У вас есть какие-нибудь планы на весенние каникулы?</t>
+  </si>
+  <si>
     <t>Grand Canyon is one of the seven wonders of the world</t>
   </si>
   <si>
-    <t>fly with three kids</t>
-  </si>
-  <si>
-    <t>to rent a car</t>
-  </si>
-  <si>
-    <t>it will take us two days</t>
-  </si>
-  <si>
-    <t>это займет у нас 2 дня</t>
-  </si>
-  <si>
-    <t>to get to our destination</t>
-  </si>
-  <si>
-    <t>добираться до метса назначения</t>
-  </si>
-  <si>
-    <t>it will take us two days to get to our destination</t>
-  </si>
-  <si>
-    <t>нам понадобится два дня, чтобы добраться до места назначения</t>
-  </si>
-  <si>
-    <t>we also booked a hotel</t>
-  </si>
-  <si>
-    <t>мы так же забронировали отель</t>
-  </si>
-  <si>
-    <t>where we can stay</t>
-  </si>
-  <si>
-    <t>где мы можем остановиться</t>
-  </si>
-  <si>
-    <t>на ночь</t>
-  </si>
-  <si>
-    <t>for the night</t>
-  </si>
-  <si>
-    <t>we also booked a hotel where we can stay for the night</t>
-  </si>
-  <si>
-    <t>мы так же забронировали отель, где мы можем остановиться на ночь</t>
-  </si>
-  <si>
-    <t>the hotel</t>
-  </si>
-  <si>
-    <t>отель</t>
-  </si>
-  <si>
-    <t>предоставляет завтрак</t>
-  </si>
-  <si>
-    <t>the hotel provides breakfast</t>
-  </si>
-  <si>
-    <t>to provides breakfast</t>
-  </si>
-  <si>
-    <t>отель предоставляет завтрак</t>
-  </si>
-  <si>
-    <t>we don’t nood to worry about</t>
-  </si>
-  <si>
-    <t>нам не нужно беспокоиться о</t>
-  </si>
-  <si>
-    <t>finding food in the morning</t>
-  </si>
-  <si>
-    <t>поиск еды на утро</t>
-  </si>
-  <si>
-    <t>we don’t need to worry about finding food in the morning</t>
-  </si>
-  <si>
-    <t>нам не унжно беспокоиться о поиске еды на утро</t>
-  </si>
-  <si>
-    <t>it is very convinient</t>
-  </si>
-  <si>
-    <t>это очень удобно</t>
-  </si>
-  <si>
-    <t>and usually</t>
-  </si>
-  <si>
-    <t>и обычно</t>
-  </si>
-  <si>
-    <t>food is quite good</t>
-  </si>
-  <si>
-    <t>еда довольно вкусная</t>
-  </si>
-  <si>
-    <t>it is very convinient, and usually, the food is quite good</t>
-  </si>
-  <si>
-    <t>это очень удобно, и обычно эта еда довольно вкусная</t>
-  </si>
-  <si>
-    <t>we can quickly eat</t>
-  </si>
-  <si>
-    <t>мы можем быстро поесть</t>
-  </si>
-  <si>
-    <t>check out</t>
-  </si>
-  <si>
-    <t>выписаться из отеля</t>
-  </si>
-  <si>
-    <t>and continue our journey</t>
-  </si>
-  <si>
-    <t>и продолжить наше путешествие</t>
-  </si>
-  <si>
-    <t>we can quickly eat, check out, and continue our journey</t>
-  </si>
-  <si>
-    <t>мы можем быстро поесть, выписаться из отеля и продолжить наше путишествие</t>
-  </si>
-  <si>
-    <t>we always plan</t>
-  </si>
-  <si>
-    <t>мы всегда планируем</t>
-  </si>
-  <si>
-    <t>a leaving early in the morning</t>
-  </si>
-  <si>
-    <t>отъезд рано утром</t>
-  </si>
-  <si>
-    <t>we have</t>
-  </si>
-  <si>
-    <t>у нас есть</t>
-  </si>
-  <si>
-    <t>we always plan on leaving early in the morning, so we have plenty of time to drive</t>
-  </si>
-  <si>
-    <t>мы всегда планируем отъезд рано утром, так, чтобы иметь достаточно времени на дорогу</t>
-  </si>
-  <si>
-    <t>but when you have children</t>
-  </si>
-  <si>
-    <t>но когда у вас есть дети</t>
-  </si>
-  <si>
-    <t>it is very difficult to leave early</t>
-  </si>
-  <si>
-    <t>это очень сложно  - выезжать рано</t>
-  </si>
-  <si>
-    <t>but when your have children, it is very difficult to leave early</t>
-  </si>
-  <si>
-    <t>но когда у вас есть дети, то сложно выезжать рано</t>
-  </si>
-  <si>
-    <t>I just hope</t>
-  </si>
-  <si>
-    <t>я просто надеюсь</t>
-  </si>
-  <si>
-    <t>we get to hotel</t>
-  </si>
-  <si>
-    <t>мы добераемся до отеля</t>
-  </si>
-  <si>
-    <t>до того, как стемнеет</t>
-  </si>
-  <si>
-    <t>I just hope we get to hotel before it gets dark</t>
-  </si>
-  <si>
-    <t>before it gets dark</t>
-  </si>
-  <si>
-    <t>it is hard to me</t>
-  </si>
-  <si>
-    <t>это сложно для меня</t>
-  </si>
-  <si>
-    <t>to drive at night</t>
-  </si>
-  <si>
-    <t>ехать ночью</t>
-  </si>
-  <si>
-    <t>it is hard to me to drive at night</t>
-  </si>
-  <si>
-    <t>это сложно для меня - ехать ночью</t>
-  </si>
-  <si>
-    <t>Do you like traveling?</t>
-  </si>
-  <si>
-    <t>вам нравится путешествовать?</t>
-  </si>
-  <si>
-    <t>plenty of time to drive</t>
-  </si>
-  <si>
-    <t>достаточно времени на дорогу</t>
+    <t>a great time</t>
+  </si>
+  <si>
+    <t>it is very expensive</t>
+  </si>
+  <si>
+    <t>we considered flying, but it is very expensive to fly with three kids</t>
+  </si>
+  <si>
+    <t>кроме того, когда мы доберемся до местоназначения</t>
+  </si>
+  <si>
+    <t>besides, when we get to our destination</t>
+  </si>
+  <si>
+    <t>нам придется арендовать машину</t>
+  </si>
+  <si>
+    <t>we would have to rent car</t>
+  </si>
+  <si>
+    <t>we would have to rent a car</t>
+  </si>
+  <si>
+    <t>besides, when we get to our destination we would have to rent a car</t>
+  </si>
+  <si>
+    <t>it is not very convinient</t>
+  </si>
+  <si>
+    <t>it is not very convinient and it is not cheap either</t>
+  </si>
+  <si>
+    <t>it takes more time and it is more tiring, but we can stop and to visit places on the way</t>
+  </si>
+  <si>
+    <t>there is not breakfast provided</t>
+  </si>
+  <si>
+    <t>we always plan on leaving early in the morning</t>
+  </si>
+  <si>
+    <t>we moved to the USA not that logn ago</t>
+  </si>
+  <si>
+    <t>it is more tiirig</t>
+  </si>
+  <si>
+    <t>we have a mini-van</t>
+  </si>
+  <si>
+    <t>we have a mini-van that has enough space for us and our luggage</t>
+  </si>
+  <si>
+    <t>eating our is not very healthy and can be also very expensive</t>
+  </si>
+  <si>
+    <t>it will takes us two days</t>
+  </si>
+  <si>
+    <t>it will take us two days to get our destination</t>
+  </si>
+  <si>
+    <t>when we can stay</t>
+  </si>
+  <si>
+    <t>we also booked a hotel when we can stay for the night</t>
+  </si>
+  <si>
+    <t>a finding food in the morning</t>
+  </si>
+  <si>
+    <t>a food is quite good</t>
+  </si>
+  <si>
+    <t>it is very convinient and usually the food is quite good</t>
+  </si>
+  <si>
+    <t>and continie our journey</t>
+  </si>
+  <si>
+    <t>we can quickly eat, check out, and continut our journey</t>
+  </si>
+  <si>
+    <t>but when you have children, it is very difficult to leave early</t>
+  </si>
+  <si>
+    <t>it is hard to me drive at nigh</t>
+  </si>
+  <si>
+    <t>это жестко для меня</t>
+  </si>
+  <si>
+    <t>try your best practice</t>
+  </si>
+  <si>
+    <t>to write your comments in English</t>
+  </si>
+  <si>
+    <t>try your best practice and write your comments in English</t>
   </si>
 </sst>
 </file>
@@ -2272,7 +2380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2295,11 +2403,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2330,8 +2488,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9755,7 +9934,7 @@
         <v>323</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="1" t="s">
@@ -9766,7 +9945,7 @@
         <v>true</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="G100" s="1" t="str">
         <f t="shared" si="3"/>
@@ -12779,10 +12958,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E8673C-6BD2-4CFE-B385-306106CCD850}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="A183" sqref="A183"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13762,32 +13941,32 @@
       <c r="A92" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="B92" s="15" t="s">
+      <c r="B92" s="16" t="s">
         <v>530</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>640</v>
+      <c r="C92" s="20" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>531</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="16" t="s">
         <v>532</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>531</v>
+      <c r="C93" s="21" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
         <v>534</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="16" t="s">
         <v>535</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="21" t="s">
         <v>534</v>
       </c>
     </row>
@@ -13795,21 +13974,21 @@
       <c r="A95" s="13" t="s">
         <v>533</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B95" s="17" t="s">
         <v>536</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>643</v>
+      <c r="C95" s="19" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
         <v>537</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="16" t="s">
         <v>538</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="20" t="s">
         <v>537</v>
       </c>
     </row>
@@ -13817,10 +13996,10 @@
       <c r="A97" s="15" t="s">
         <v>539</v>
       </c>
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="16" t="s">
         <v>540</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="21" t="s">
         <v>539</v>
       </c>
     </row>
@@ -13828,54 +14007,54 @@
       <c r="A98" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="B98" s="13" t="s">
+      <c r="B98" s="17" t="s">
         <v>542</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>541</v>
+      <c r="C98" s="19" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>641</v>
-      </c>
-      <c r="B99" s="15" t="s">
+        <v>627</v>
+      </c>
+      <c r="B99" s="16" t="s">
         <v>543</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>641</v>
+      <c r="C99" s="20" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
         <v>544</v>
       </c>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="21" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>644</v>
-      </c>
-      <c r="B101" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="B101" s="17" t="s">
         <v>546</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>644</v>
+      <c r="C101" s="19" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
         <v>547</v>
       </c>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="20" t="s">
         <v>547</v>
       </c>
     </row>
@@ -13883,10 +14062,10 @@
       <c r="A103" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="B103" s="15" t="s">
+      <c r="B103" s="16" t="s">
         <v>550</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="21" t="s">
         <v>549</v>
       </c>
     </row>
@@ -13894,32 +14073,32 @@
       <c r="A104" s="15" t="s">
         <v>551</v>
       </c>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="16" t="s">
         <v>552</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>642</v>
+      <c r="C104" s="21" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>553</v>
       </c>
-      <c r="B105" s="13" t="s">
+      <c r="B105" s="17" t="s">
         <v>554</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>645</v>
+      <c r="C105" s="19" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>555</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B106" s="16" t="s">
         <v>556</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="20" t="s">
         <v>555</v>
       </c>
     </row>
@@ -13927,691 +14106,924 @@
       <c r="A107" s="15" t="s">
         <v>557</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="16" t="s">
         <v>559</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>557</v>
+      <c r="C107" s="21" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
         <v>558</v>
       </c>
-      <c r="B108" s="15" t="s">
+      <c r="B108" s="16" t="s">
         <v>560</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>646</v>
+      <c r="C108" s="21" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>561</v>
       </c>
-      <c r="B109" s="13" t="s">
-        <v>562</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>561</v>
+      <c r="B109" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
+        <v>562</v>
+      </c>
+      <c r="B110" s="16" t="s">
         <v>563</v>
       </c>
-      <c r="B110" s="15" t="s">
-        <v>564</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>563</v>
+      <c r="C110" s="21" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
-        <v>565</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="C111" s="21" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="B112" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="C112" s="21" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>569</v>
-      </c>
-      <c r="B113" s="13" t="s">
-        <v>580</v>
-      </c>
-      <c r="C113" s="16" t="s">
-        <v>569</v>
+        <v>568</v>
+      </c>
+      <c r="B113" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="C113" s="22" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="B114" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="B114" s="15" t="s">
-        <v>571</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>570</v>
+      <c r="C114" s="21" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>573</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>572</v>
+        <v>727</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>726</v>
+      </c>
+      <c r="C115" s="21" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="B116" s="15" t="s">
-        <v>575</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="C116" s="21" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>576</v>
-      </c>
-      <c r="B117" s="15" t="s">
-        <v>577</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>647</v>
+        <v>729</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>728</v>
+      </c>
+      <c r="C117" s="21" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>578</v>
-      </c>
-      <c r="B118" s="13" t="s">
-        <v>579</v>
-      </c>
-      <c r="C118" s="16" t="s">
-        <v>578</v>
+        <v>573</v>
+      </c>
+      <c r="B118" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="C118" s="22" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
-        <v>581</v>
-      </c>
-      <c r="B119" s="15" t="s">
-        <v>582</v>
+        <v>576</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>583</v>
-      </c>
-      <c r="B120" s="15" t="s">
-        <v>586</v>
+        <v>578</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>584</v>
-      </c>
-      <c r="B121" s="13" t="s">
-        <v>585</v>
+        <v>579</v>
+      </c>
+      <c r="B121" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="C121" s="18" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="15" t="s">
-        <v>587</v>
-      </c>
-      <c r="B122" s="15" t="s">
-        <v>588</v>
+      <c r="A122" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="B122" s="13" t="s">
+        <v>583</v>
+      </c>
+      <c r="C122" s="19" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
-        <v>589</v>
-      </c>
-      <c r="B123" s="15" t="s">
-        <v>590</v>
+        <v>584</v>
+      </c>
+      <c r="B123" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="C123" s="20" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="13" t="s">
-        <v>591</v>
-      </c>
-      <c r="B124" s="13" t="s">
-        <v>592</v>
+      <c r="A124" s="15" t="s">
+        <v>586</v>
+      </c>
+      <c r="B124" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
-        <v>593</v>
-      </c>
-      <c r="B125" s="15" t="s">
-        <v>594</v>
+        <v>588</v>
+      </c>
+      <c r="B125" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="C125" s="21" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>595</v>
-      </c>
-      <c r="B126" s="15" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="15" t="s">
-        <v>597</v>
-      </c>
-      <c r="B127" s="15" t="s">
-        <v>598</v>
+        <v>705</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="C126" s="21" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="13" t="s">
+        <v>707</v>
+      </c>
+      <c r="B127" s="17" t="s">
+        <v>591</v>
+      </c>
+      <c r="C127" s="22" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="B128" s="15" t="s">
+        <v>593</v>
+      </c>
+      <c r="C128" s="20" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="B129" s="15" t="s">
+        <v>595</v>
+      </c>
+      <c r="C129" s="21" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="15" t="s">
+        <v>708</v>
+      </c>
+      <c r="B130" s="15" t="s">
+        <v>596</v>
+      </c>
+      <c r="C130" s="21" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="13" t="s">
+        <v>709</v>
+      </c>
+      <c r="B131" s="13" t="s">
+        <v>597</v>
+      </c>
+      <c r="C131" s="18" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="15" t="s">
+        <v>598</v>
+      </c>
+      <c r="B132" s="15" t="s">
         <v>599</v>
       </c>
-      <c r="B128" s="15" t="s">
+      <c r="C132" s="20" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="15" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="13" t="s">
+      <c r="B133" s="15" t="s">
         <v>601</v>
       </c>
-      <c r="B129" s="13" t="s">
+      <c r="C133" s="21" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="15" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="15" t="s">
+      <c r="B134" s="15" t="s">
         <v>603</v>
       </c>
-      <c r="B130" s="15" t="s">
+      <c r="C134" s="21" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="13" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="15" t="s">
+      <c r="B135" s="13" t="s">
         <v>605</v>
       </c>
-      <c r="B131" s="15" t="s">
+      <c r="C135" s="18" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="15" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="15" t="s">
+      <c r="B136" s="15" t="s">
         <v>607</v>
       </c>
-      <c r="B132" s="15" t="s">
+      <c r="C136" s="20" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="15" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A133" s="13" t="s">
+      <c r="B137" s="15" t="s">
         <v>609</v>
       </c>
-      <c r="B133" s="13" t="s">
+      <c r="C137" s="21" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="13" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="15" t="s">
+      <c r="B138" s="13" t="s">
         <v>611</v>
       </c>
-      <c r="B134" s="15" t="s">
+      <c r="C138" s="18" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="15" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="15" t="s">
+      <c r="B139" s="15" t="s">
         <v>613</v>
       </c>
-      <c r="B135" s="15" t="s">
+      <c r="C139" s="20" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="15" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="15" t="s">
+      <c r="B140" s="15" t="s">
         <v>615</v>
       </c>
-      <c r="B136" s="15" t="s">
+      <c r="C140" s="21" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="13" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="13" t="s">
+      <c r="B141" s="13" t="s">
         <v>617</v>
       </c>
-      <c r="B137" s="13" t="s">
+      <c r="C141" s="18" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="15" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="15" t="s">
+      <c r="B142" s="15" t="s">
         <v>619</v>
       </c>
-      <c r="B138" s="15" t="s">
+      <c r="C142" s="20" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="15" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="15" t="s">
+      <c r="B143" s="15" t="s">
         <v>621</v>
       </c>
-      <c r="B139" s="15" t="s">
+      <c r="C143" s="21" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="15" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A140" s="13" t="s">
+      <c r="B144" s="15" t="s">
         <v>623</v>
       </c>
-      <c r="B140" s="13" t="s">
+      <c r="C144" s="21" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="13" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="15" t="s">
+      <c r="B145" s="13" t="s">
         <v>625</v>
       </c>
-      <c r="B141" s="15" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="15" t="s">
-        <v>627</v>
-      </c>
-      <c r="B142" s="15" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="13" t="s">
-        <v>629</v>
-      </c>
-      <c r="B143" s="13" t="s">
+      <c r="C145" s="18" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="15" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="15" t="s">
+      <c r="B146" s="15" t="s">
         <v>631</v>
       </c>
-      <c r="B144" s="15" t="s">
+      <c r="C146" s="20" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="15" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="15" t="s">
+      <c r="B147" s="15" t="s">
         <v>633</v>
       </c>
-      <c r="B145" s="15" t="s">
+      <c r="C147" s="21" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="13" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="15" t="s">
+      <c r="B148" s="13" t="s">
         <v>635</v>
       </c>
-      <c r="B146" s="15" t="s">
+      <c r="C148" s="18" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="15" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="13" t="s">
+      <c r="B149" s="15" t="s">
         <v>637</v>
       </c>
-      <c r="B147" s="13" t="s">
+      <c r="C149" s="20" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="15" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="15" t="s">
+      <c r="B150" s="15" t="s">
+        <v>639</v>
+      </c>
+      <c r="C150" s="21" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="15" t="s">
+        <v>641</v>
+      </c>
+      <c r="B151" s="15" t="s">
+        <v>640</v>
+      </c>
+      <c r="C151" s="21" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="13" t="s">
+        <v>642</v>
+      </c>
+      <c r="B152" s="13" t="s">
+        <v>643</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="13" t="s">
+        <v>644</v>
+      </c>
+      <c r="B153" s="13" t="s">
+        <v>645</v>
+      </c>
+      <c r="C153" s="18" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="15" t="s">
+        <v>710</v>
+      </c>
+      <c r="B154" s="15" t="s">
+        <v>646</v>
+      </c>
+      <c r="C154" s="20" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="B155" s="15" t="s">
         <v>648</v>
       </c>
-      <c r="B148" s="15" t="s">
+      <c r="C155" s="21" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="13" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="15" t="s">
+      <c r="B156" s="13" t="s">
         <v>650</v>
       </c>
-      <c r="B149" s="15" t="s">
+      <c r="C156" s="18" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="15" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="13" t="s">
+      <c r="B157" s="15" t="s">
         <v>652</v>
       </c>
-      <c r="B150" s="13" t="s">
+      <c r="C157" s="20" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="15" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="15" t="s">
+      <c r="B158" s="15" t="s">
         <v>654</v>
       </c>
-      <c r="B151" s="15" t="s">
+      <c r="C158" s="21" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="15" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="15" t="s">
+      <c r="B159" s="15" t="s">
         <v>656</v>
       </c>
-      <c r="B152" s="15" t="s">
+      <c r="C159" s="21" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="13" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="15" t="s">
+      <c r="B160" s="13" t="s">
+        <v>711</v>
+      </c>
+      <c r="C160" s="18" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="15" t="s">
+        <v>658</v>
+      </c>
+      <c r="B161" s="15" t="s">
         <v>659</v>
       </c>
-      <c r="B153" s="15" t="s">
+      <c r="C161" s="20" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="13" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="15" t="s">
         <v>660</v>
       </c>
-      <c r="B154" s="13" t="s">
+      <c r="B162" s="15" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="15" t="s">
+      <c r="C162" s="21" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="15" t="s">
         <v>662</v>
       </c>
-      <c r="B155" s="15" t="s">
+      <c r="B163" s="15" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="15" t="s">
+      <c r="C163" s="21" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="13" t="s">
+        <v>664</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>665</v>
+      </c>
+      <c r="C164" s="18" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="15" t="s">
         <v>666</v>
       </c>
-      <c r="B156" s="15" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="13" t="s">
-        <v>665</v>
-      </c>
-      <c r="B157" s="13" t="s">
+      <c r="B165" s="15" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="15" t="s">
+      <c r="C165" s="20" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="15" t="s">
+        <v>715</v>
+      </c>
+      <c r="B166" s="15" t="s">
+        <v>714</v>
+      </c>
+      <c r="C166" s="21" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="15" t="s">
+        <v>716</v>
+      </c>
+      <c r="B167" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="C167" s="21" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="B168" s="15" t="s">
+        <v>713</v>
+      </c>
+      <c r="C168" s="21" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="13" t="s">
         <v>668</v>
       </c>
-      <c r="B158" s="15" t="s">
+      <c r="B169" s="13" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="15" t="s">
+      <c r="C169" s="22" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="15" t="s">
         <v>670</v>
       </c>
-      <c r="B159" s="15" t="s">
+      <c r="B170" s="15" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="13" t="s">
+      <c r="C170" s="20" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="15" t="s">
         <v>672</v>
       </c>
-      <c r="B160" s="13" t="s">
+      <c r="B171" s="15" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="15" t="s">
+      <c r="C171" s="21" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="13" t="s">
         <v>674</v>
       </c>
-      <c r="B161" s="15" t="s">
+      <c r="B172" s="13" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="15" t="s">
+      <c r="C172" s="18" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="15" t="s">
         <v>676</v>
       </c>
-      <c r="B162" s="15" t="s">
+      <c r="B173" s="15" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="15" t="s">
+      <c r="C173" s="20" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="15" t="s">
         <v>678</v>
       </c>
-      <c r="B163" s="15" t="s">
+      <c r="B174" s="15" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="13" t="s">
+      <c r="C174" s="21" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="15" t="s">
+        <v>720</v>
+      </c>
+      <c r="B175" s="15" t="s">
+        <v>719</v>
+      </c>
+      <c r="C175" s="21" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="13" t="s">
         <v>680</v>
       </c>
-      <c r="B164" s="13" t="s">
+      <c r="B176" s="13" t="s">
+        <v>718</v>
+      </c>
+      <c r="C176" s="18" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="15" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="15" t="s">
+      <c r="B177" s="15" t="s">
+        <v>753</v>
+      </c>
+      <c r="C177" s="20" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="15" t="s">
         <v>682</v>
       </c>
-      <c r="B165" s="15" t="s">
+      <c r="B178" s="15" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="15" t="s">
+      <c r="C178" s="21" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="B166" s="15" t="s">
+      <c r="B179" s="13" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="15" t="s">
+      <c r="C179" s="18" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="13" t="s">
+        <v>687</v>
+      </c>
+      <c r="B180" s="13" t="s">
         <v>686</v>
       </c>
-      <c r="B167" s="15" t="s">
+      <c r="C180" s="23" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="13" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="13" t="s">
         <v>688</v>
       </c>
-      <c r="B168" s="13" t="s">
+      <c r="B181" s="13" t="s">
+        <v>721</v>
+      </c>
+      <c r="C181" s="23" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="13" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="15" t="s">
+      <c r="B182" s="13" t="s">
         <v>690</v>
       </c>
-      <c r="B169" s="15" t="s">
+      <c r="C182" s="23" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="15" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="15" t="s">
+      <c r="B183" s="15" t="s">
         <v>692</v>
       </c>
-      <c r="B170" s="15" t="s">
+      <c r="C183" s="20" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="15" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="15" t="s">
+      <c r="B184" s="15" t="s">
         <v>694</v>
       </c>
-      <c r="B171" s="15" t="s">
+      <c r="C184" s="21" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="13" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="15" t="s">
-        <v>719</v>
-      </c>
-      <c r="B172" s="15" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="13" t="s">
+      <c r="B185" s="13" t="s">
         <v>696</v>
       </c>
-      <c r="B173" s="13" t="s">
+      <c r="C185" s="18" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="13" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="15" t="s">
+      <c r="B186" s="13" t="s">
         <v>698</v>
       </c>
-      <c r="B174" s="15" t="s">
+      <c r="C186" s="23" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="15" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="15" t="s">
+      <c r="B187" s="15" t="s">
         <v>700</v>
       </c>
-      <c r="B175" s="15" t="s">
+      <c r="C187" s="20" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="15" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="13" t="s">
+      <c r="B188" s="15" t="s">
         <v>702</v>
       </c>
-      <c r="B176" s="13" t="s">
+      <c r="C188" s="21" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="13" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="15" t="s">
+      <c r="B189" s="13" t="s">
         <v>704</v>
       </c>
-      <c r="B177" s="15" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="15" t="s">
-        <v>706</v>
-      </c>
-      <c r="B178" s="15" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="15" t="s">
-        <v>710</v>
-      </c>
-      <c r="B179" s="15" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="13" t="s">
-        <v>709</v>
-      </c>
-      <c r="B180" s="13" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="15" t="s">
-        <v>711</v>
-      </c>
-      <c r="B181" s="15" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="15" t="s">
-        <v>713</v>
-      </c>
-      <c r="B182" s="15" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="13" t="s">
-        <v>715</v>
-      </c>
-      <c r="B183" s="13" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="13" t="s">
-        <v>717</v>
-      </c>
-      <c r="B184" s="13" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="13"/>
-      <c r="B185" s="13"/>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="13"/>
-      <c r="B186" s="13"/>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="13"/>
-      <c r="B187" s="13"/>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="13"/>
-      <c r="B188" s="13"/>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="13"/>
-      <c r="B189" s="13"/>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C189" s="18" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="13"/>
       <c r="B190" s="13"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
       <c r="B191" s="13"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="13"/>
       <c r="B192" s="13"/>
     </row>
@@ -14626,22 +15038,6 @@
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="13"/>
       <c r="B195" s="13"/>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="13"/>
-      <c r="B196" s="13"/>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="13"/>
-      <c r="B197" s="13"/>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="13"/>
-      <c r="B198" s="13"/>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="13"/>
-      <c r="B199" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add continue history of secret of happy life
</commit_message>
<xml_diff>
--- a/english.xlsx
+++ b/english.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="979">
   <si>
     <t>word</t>
   </si>
@@ -2714,6 +2714,255 @@
   </si>
   <si>
     <t>во-первых, ты должен проводить больше времени на рыбалке, так ты можешь поймать больше рыбы - начал бизнесмен</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>that would be easy to do</t>
+  </si>
+  <si>
+    <t>said fisherman</t>
+  </si>
+  <si>
+    <t>ok, that would be easy to do - said fisherman</t>
+  </si>
+  <si>
+    <t>это будет легко сделать</t>
+  </si>
+  <si>
+    <t>сказал рыбак</t>
+  </si>
+  <si>
+    <t>хорошо, это будет легко сделать - сказал рыбак</t>
+  </si>
+  <si>
+    <t>the businessman nodded in agreement</t>
+  </si>
+  <si>
+    <t>бизнесмен кивнул в знак согласия</t>
+  </si>
+  <si>
+    <t>and buy a bigger boat</t>
+  </si>
+  <si>
+    <t>и купить более большую лодку</t>
+  </si>
+  <si>
+    <t>continued the businessman</t>
+  </si>
+  <si>
+    <t>продолжил бизнесмен</t>
+  </si>
+  <si>
+    <t>you can then</t>
+  </si>
+  <si>
+    <t>you can then sell the extra fish</t>
+  </si>
+  <si>
+    <t>затем ты сможешь</t>
+  </si>
+  <si>
+    <t>затем ты сможешь продавать дополнительную рыбу</t>
+  </si>
+  <si>
+    <t>you can then sell the extra fish and buy a bigger boat - continued businessman</t>
+  </si>
+  <si>
+    <t>затем ты сможешь продавать дополнительную рыбу и купить более большую лодку - продолжил бизнесмен</t>
+  </si>
+  <si>
+    <t>what for</t>
+  </si>
+  <si>
+    <t>зачем</t>
+  </si>
+  <si>
+    <t>asked the fisherman</t>
+  </si>
+  <si>
+    <t>спросил рыбак</t>
+  </si>
+  <si>
+    <t>asked the fisherman very politely</t>
+  </si>
+  <si>
+    <t>what for - asked the fisherman very politely</t>
+  </si>
+  <si>
+    <t>спросил рыбае очень вежливо</t>
+  </si>
+  <si>
+    <t>зачем - спросил рыбак очень вежливо</t>
+  </si>
+  <si>
+    <t>with a bigger boat</t>
+  </si>
+  <si>
+    <t>с более большой лодкой</t>
+  </si>
+  <si>
+    <t>you will catch even more fish</t>
+  </si>
+  <si>
+    <t>ты поймаешь еще больше рыбы</t>
+  </si>
+  <si>
+    <t>said the businessman</t>
+  </si>
+  <si>
+    <t>with a bigger boat, you will catch even more fish - said businessman</t>
+  </si>
+  <si>
+    <t>с более большой лодкой, ты поймаешь еще больше рыбы - сказал бизнесмен</t>
+  </si>
+  <si>
+    <t>soon</t>
+  </si>
+  <si>
+    <t>скоро</t>
+  </si>
+  <si>
+    <t>you will be able</t>
+  </si>
+  <si>
+    <t>ты сможешь</t>
+  </si>
+  <si>
+    <t>to buy another boat</t>
+  </si>
+  <si>
+    <t>купить другую лодку</t>
+  </si>
+  <si>
+    <t>hire people</t>
+  </si>
+  <si>
+    <t>нанять людей</t>
+  </si>
+  <si>
+    <t>and build a big business</t>
+  </si>
+  <si>
+    <t>и построить большой бизнес</t>
+  </si>
+  <si>
+    <t>soon you will be able to by another boat, hire people, and build a big business</t>
+  </si>
+  <si>
+    <t>скоро, ты сможешь купить другую лодку, нанять людей, и построить большой бизнес</t>
+  </si>
+  <si>
+    <t>the businessman was very excided</t>
+  </si>
+  <si>
+    <t>бизнесмен был очень взволнован</t>
+  </si>
+  <si>
+    <t>когда</t>
+  </si>
+  <si>
+    <t>ones</t>
+  </si>
+  <si>
+    <t>your business is big enough</t>
+  </si>
+  <si>
+    <t>твой бизнес станет достаточно большим</t>
+  </si>
+  <si>
+    <t>you can sell it</t>
+  </si>
+  <si>
+    <t>ты можешь продать его</t>
+  </si>
+  <si>
+    <t>and make a lot of money</t>
+  </si>
+  <si>
+    <t>и заработать много денег</t>
+  </si>
+  <si>
+    <t>ones your business is big enough, you can sell it and make a lot of money</t>
+  </si>
+  <si>
+    <t>когда твой бизнес станет достаточно большим, ты сможешь продать его, и заработать много денег</t>
+  </si>
+  <si>
+    <t>that sounds great</t>
+  </si>
+  <si>
+    <t>звучит здорово</t>
+  </si>
+  <si>
+    <t>said the fisherman</t>
+  </si>
+  <si>
+    <t>that sounds great - said the fisherman</t>
+  </si>
+  <si>
+    <t>звучит здорово - сказал рыбак</t>
+  </si>
+  <si>
+    <t>and what then</t>
+  </si>
+  <si>
+    <t>и что потом</t>
+  </si>
+  <si>
+    <t>then</t>
+  </si>
+  <si>
+    <t>затем</t>
+  </si>
+  <si>
+    <t>you can retire</t>
+  </si>
+  <si>
+    <t>ты сможешь уйти на пенсию</t>
+  </si>
+  <si>
+    <t>spend time with your family</t>
+  </si>
+  <si>
+    <t>play the guitar</t>
+  </si>
+  <si>
+    <t>and enjoy life with your friends</t>
+  </si>
+  <si>
+    <t>then, you can retire, spend time with your family, play the guitar, and enjoy life with your friends - said the businessman</t>
+  </si>
+  <si>
+    <t>проводить время со своей семьей</t>
+  </si>
+  <si>
+    <t>играть на гитаре</t>
+  </si>
+  <si>
+    <t>и радоваться жизни со своими друзьями</t>
+  </si>
+  <si>
+    <t>затем, ты можешь уйти на пенсию, проводить время с семьей, играть на гитаре, радоваться жизни со своими друзьями - сказал бизнесмен</t>
+  </si>
+  <si>
+    <t>the fisherman smiled and said</t>
+  </si>
+  <si>
+    <t>рыбал улыбнулся и сказал</t>
+  </si>
+  <si>
+    <t>is not that what I am doing right now</t>
+  </si>
+  <si>
+    <t>разве это не то, что я делаю прямо сейчас</t>
+  </si>
+  <si>
+    <t>the fisherman smiled and said - is not thar what I am doing right now</t>
+  </si>
+  <si>
+    <t>рыбак улыбнулся и сказал - разве это не то, что делаю прямо сейчас</t>
   </si>
 </sst>
 </file>
@@ -13379,8 +13628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="A258" sqref="A258"/>
+    <sheetView tabSelected="1" topLeftCell="A284" workbookViewId="0">
+      <selection activeCell="A305" sqref="A305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16001,180 +16250,356 @@
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A261" s="13"/>
-      <c r="B261" s="13"/>
+      <c r="A261" s="13" t="s">
+        <v>896</v>
+      </c>
+      <c r="B261" s="13" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A262" s="13"/>
-      <c r="B262" s="13"/>
+      <c r="A262" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="B262" s="13" t="s">
+        <v>900</v>
+      </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A263" s="13"/>
-      <c r="B263" s="13"/>
+      <c r="A263" s="13" t="s">
+        <v>898</v>
+      </c>
+      <c r="B263" s="13" t="s">
+        <v>901</v>
+      </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A264" s="13"/>
-      <c r="B264" s="13"/>
+      <c r="A264" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="B264" s="15" t="s">
+        <v>902</v>
+      </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A265" s="13"/>
-      <c r="B265" s="13"/>
+      <c r="A265" s="15" t="s">
+        <v>903</v>
+      </c>
+      <c r="B265" s="15" t="s">
+        <v>904</v>
+      </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A266" s="13"/>
-      <c r="B266" s="13"/>
+      <c r="A266" s="13" t="s">
+        <v>909</v>
+      </c>
+      <c r="B266" s="13" t="s">
+        <v>911</v>
+      </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A267" s="13"/>
-      <c r="B267" s="13"/>
+      <c r="A267" s="13" t="s">
+        <v>910</v>
+      </c>
+      <c r="B267" s="13" t="s">
+        <v>912</v>
+      </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A268" s="13"/>
-      <c r="B268" s="13"/>
+      <c r="A268" s="13" t="s">
+        <v>905</v>
+      </c>
+      <c r="B268" s="13" t="s">
+        <v>906</v>
+      </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A269" s="13"/>
-      <c r="B269" s="13"/>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A270" s="13"/>
-      <c r="B270" s="13"/>
+      <c r="A269" s="13" t="s">
+        <v>907</v>
+      </c>
+      <c r="B269" s="13" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A270" s="15" t="s">
+        <v>913</v>
+      </c>
+      <c r="B270" s="15" t="s">
+        <v>914</v>
+      </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A271" s="13"/>
-      <c r="B271" s="13"/>
+      <c r="A271" s="13" t="s">
+        <v>915</v>
+      </c>
+      <c r="B271" s="13" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A272" s="13"/>
-      <c r="B272" s="13"/>
+      <c r="A272" s="13" t="s">
+        <v>917</v>
+      </c>
+      <c r="B272" s="13" t="s">
+        <v>918</v>
+      </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A273" s="13"/>
-      <c r="B273" s="13"/>
+      <c r="A273" s="13" t="s">
+        <v>919</v>
+      </c>
+      <c r="B273" s="13" t="s">
+        <v>921</v>
+      </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A274" s="13"/>
-      <c r="B274" s="13"/>
+      <c r="A274" s="15" t="s">
+        <v>920</v>
+      </c>
+      <c r="B274" s="15" t="s">
+        <v>922</v>
+      </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A275" s="13"/>
-      <c r="B275" s="13"/>
+      <c r="A275" s="13" t="s">
+        <v>923</v>
+      </c>
+      <c r="B275" s="13" t="s">
+        <v>924</v>
+      </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A276" s="13"/>
-      <c r="B276" s="13"/>
+      <c r="A276" s="13" t="s">
+        <v>925</v>
+      </c>
+      <c r="B276" s="13" t="s">
+        <v>926</v>
+      </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A277" s="13"/>
-      <c r="B277" s="13"/>
+      <c r="A277" s="13" t="s">
+        <v>927</v>
+      </c>
+      <c r="B277" s="13" t="s">
+        <v>871</v>
+      </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A278" s="13"/>
-      <c r="B278" s="13"/>
+      <c r="A278" s="15" t="s">
+        <v>928</v>
+      </c>
+      <c r="B278" s="15" t="s">
+        <v>929</v>
+      </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A279" s="13"/>
-      <c r="B279" s="13"/>
+      <c r="A279" s="13" t="s">
+        <v>930</v>
+      </c>
+      <c r="B279" s="13" t="s">
+        <v>931</v>
+      </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A280" s="13"/>
-      <c r="B280" s="13"/>
+      <c r="A280" s="13" t="s">
+        <v>932</v>
+      </c>
+      <c r="B280" s="13" t="s">
+        <v>933</v>
+      </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A281" s="13"/>
-      <c r="B281" s="13"/>
+      <c r="A281" s="13" t="s">
+        <v>934</v>
+      </c>
+      <c r="B281" s="13" t="s">
+        <v>935</v>
+      </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A282" s="13"/>
-      <c r="B282" s="13"/>
+      <c r="A282" s="13" t="s">
+        <v>936</v>
+      </c>
+      <c r="B282" s="13" t="s">
+        <v>937</v>
+      </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A283" s="13"/>
-      <c r="B283" s="13"/>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A284" s="13"/>
-      <c r="B284" s="13"/>
+      <c r="A283" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="B283" s="13" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A284" s="15" t="s">
+        <v>940</v>
+      </c>
+      <c r="B284" s="15" t="s">
+        <v>941</v>
+      </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A285" s="13"/>
-      <c r="B285" s="13"/>
+      <c r="A285" s="15" t="s">
+        <v>942</v>
+      </c>
+      <c r="B285" s="15" t="s">
+        <v>943</v>
+      </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A286" s="13"/>
-      <c r="B286" s="13"/>
+      <c r="A286" s="13" t="s">
+        <v>945</v>
+      </c>
+      <c r="B286" s="13" t="s">
+        <v>944</v>
+      </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A287" s="13"/>
-      <c r="B287" s="13"/>
+      <c r="A287" s="13" t="s">
+        <v>946</v>
+      </c>
+      <c r="B287" s="13" t="s">
+        <v>947</v>
+      </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A288" s="13"/>
-      <c r="B288" s="13"/>
+      <c r="A288" s="13" t="s">
+        <v>948</v>
+      </c>
+      <c r="B288" s="13" t="s">
+        <v>949</v>
+      </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A289" s="13"/>
-      <c r="B289" s="13"/>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A290" s="13"/>
-      <c r="B290" s="13"/>
+      <c r="A289" s="13" t="s">
+        <v>950</v>
+      </c>
+      <c r="B289" s="13" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A290" s="15" t="s">
+        <v>952</v>
+      </c>
+      <c r="B290" s="15" t="s">
+        <v>953</v>
+      </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A291" s="13"/>
-      <c r="B291" s="13"/>
+      <c r="A291" s="13" t="s">
+        <v>954</v>
+      </c>
+      <c r="B291" s="13" t="s">
+        <v>955</v>
+      </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A292" s="13"/>
-      <c r="B292" s="13"/>
+      <c r="A292" s="13" t="s">
+        <v>956</v>
+      </c>
+      <c r="B292" s="13" t="s">
+        <v>901</v>
+      </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A293" s="13"/>
-      <c r="B293" s="13"/>
+      <c r="A293" s="15" t="s">
+        <v>957</v>
+      </c>
+      <c r="B293" s="15" t="s">
+        <v>958</v>
+      </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A294" s="13"/>
-      <c r="B294" s="13"/>
+      <c r="A294" s="15" t="s">
+        <v>959</v>
+      </c>
+      <c r="B294" s="15" t="s">
+        <v>960</v>
+      </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A295" s="13"/>
-      <c r="B295" s="13"/>
+      <c r="A295" s="13" t="s">
+        <v>961</v>
+      </c>
+      <c r="B295" s="13" t="s">
+        <v>962</v>
+      </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A296" s="13"/>
-      <c r="B296" s="13"/>
+      <c r="A296" s="13" t="s">
+        <v>963</v>
+      </c>
+      <c r="B296" s="13" t="s">
+        <v>964</v>
+      </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A297" s="13"/>
-      <c r="B297" s="13"/>
+      <c r="A297" s="13" t="s">
+        <v>965</v>
+      </c>
+      <c r="B297" s="13" t="s">
+        <v>969</v>
+      </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A298" s="13"/>
-      <c r="B298" s="13"/>
+      <c r="A298" s="13" t="s">
+        <v>966</v>
+      </c>
+      <c r="B298" s="13" t="s">
+        <v>970</v>
+      </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A299" s="13"/>
-      <c r="B299" s="13"/>
+      <c r="A299" s="13" t="s">
+        <v>967</v>
+      </c>
+      <c r="B299" s="13" t="s">
+        <v>971</v>
+      </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A300" s="13"/>
-      <c r="B300" s="13"/>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A301" s="13"/>
-      <c r="B301" s="13"/>
+      <c r="A300" s="13" t="s">
+        <v>927</v>
+      </c>
+      <c r="B300" s="13" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A301" s="15" t="s">
+        <v>968</v>
+      </c>
+      <c r="B301" s="15" t="s">
+        <v>972</v>
+      </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A302" s="13"/>
-      <c r="B302" s="13"/>
+      <c r="A302" s="13" t="s">
+        <v>973</v>
+      </c>
+      <c r="B302" s="13" t="s">
+        <v>974</v>
+      </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A303" s="13"/>
-      <c r="B303" s="13"/>
+      <c r="A303" s="13" t="s">
+        <v>975</v>
+      </c>
+      <c r="B303" s="13" t="s">
+        <v>976</v>
+      </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A304" s="13"/>
-      <c r="B304" s="13"/>
+      <c r="A304" s="15" t="s">
+        <v>977</v>
+      </c>
+      <c r="B304" s="15" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" s="13"/>

</xml_diff>

<commit_message>
Add repeat for second story
</commit_message>
<xml_diff>
--- a/english.xlsx
+++ b/english.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popoves\Desktop\experience\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DC8081-B8A1-4C87-833C-D1B5BFF093AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77A4024-6787-4FB1-8359-4803BAE6D664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="words" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="1059">
   <si>
     <t>word</t>
   </si>
@@ -2565,12 +2565,6 @@
     <t>why don’t you stay out</t>
   </si>
   <si>
-    <t>почему бы тебе не оставаться подольше</t>
-  </si>
-  <si>
-    <t>почему бы тебе не оставаться</t>
-  </si>
-  <si>
     <t>why don’t you stay out longer</t>
   </si>
   <si>
@@ -2580,9 +2574,6 @@
     <t>и ловить больше рыбы</t>
   </si>
   <si>
-    <t>why don’t you stays out longer and catch more fish</t>
-  </si>
-  <si>
     <t>почему бы тебе не оставаться подольше и ловить больше рыбы</t>
   </si>
   <si>
@@ -2790,15 +2781,6 @@
     <t>asked the fisherman very politely</t>
   </si>
   <si>
-    <t>what for - asked the fisherman very politely</t>
-  </si>
-  <si>
-    <t>спросил рыбае очень вежливо</t>
-  </si>
-  <si>
-    <t>зачем - спросил рыбак очень вежливо</t>
-  </si>
-  <si>
     <t>with a bigger boat</t>
   </si>
   <si>
@@ -2907,12 +2889,6 @@
     <t>звучит здорово - сказал рыбак</t>
   </si>
   <si>
-    <t>and what then</t>
-  </si>
-  <si>
-    <t>и что потом</t>
-  </si>
-  <si>
     <t>then</t>
   </si>
   <si>
@@ -2952,9 +2928,6 @@
     <t>the fisherman smiled and said</t>
   </si>
   <si>
-    <t>рыбал улыбнулся и сказал</t>
-  </si>
-  <si>
     <t>is not that what I am doing right now</t>
   </si>
   <si>
@@ -3121,6 +3094,117 @@
   </si>
   <si>
     <t>если django установлен, вы увидите версию вашей установки</t>
+  </si>
+  <si>
+    <t>the routine of local fisherman</t>
+  </si>
+  <si>
+    <t>he could not help but notice the rountine of local fisherman</t>
+  </si>
+  <si>
+    <t>an ameriacan businessman</t>
+  </si>
+  <si>
+    <t>an ameriacan businessman was on vacation in Mexico</t>
+  </si>
+  <si>
+    <t>he would fish a couple hours</t>
+  </si>
+  <si>
+    <t>he would fish a couple hours and then return home with some fish</t>
+  </si>
+  <si>
+    <t>also he would give some fish to his neighbour</t>
+  </si>
+  <si>
+    <t>the businessman noticed that in the afternoon fisherman didn’t work</t>
+  </si>
+  <si>
+    <t>and enjoyed the company of his friends and neibours</t>
+  </si>
+  <si>
+    <t>instead, he spent time with his family, played the guitar, and enjoyed the company of his friends and neighbours</t>
+  </si>
+  <si>
+    <t>the businessman approached to fisherman</t>
+  </si>
+  <si>
+    <t>one day, the businessman approached to fisherman and said</t>
+  </si>
+  <si>
+    <t>I notcied</t>
+  </si>
+  <si>
+    <t>why don’t you stay out longer and catch more fish?</t>
+  </si>
+  <si>
+    <t>why don’t you stays out longer and catch more fish?</t>
+  </si>
+  <si>
+    <t>why don’t you stay out longer?</t>
+  </si>
+  <si>
+    <t>why don’t you stay out?</t>
+  </si>
+  <si>
+    <t>почему бы тебе не оставаться?</t>
+  </si>
+  <si>
+    <t>почему бы тебе не оставаться подольше?</t>
+  </si>
+  <si>
+    <t>I catch enough to support my family and little more to share with friends</t>
+  </si>
+  <si>
+    <t>I had great success building many businnes back home</t>
+  </si>
+  <si>
+    <t>first, you have to spend more time fishing, so you can catch more fish, started businessman</t>
+  </si>
+  <si>
+    <t>ok, that would be easy to do</t>
+  </si>
+  <si>
+    <t>you can then to sell extra fish and buy a bigger boat - continued businessman</t>
+  </si>
+  <si>
+    <t>спросил рыбак очень вежливо</t>
+  </si>
+  <si>
+    <t>what for? asked the fisherman very politely</t>
+  </si>
+  <si>
+    <t>зачем? спросил рыбак очень вежливо</t>
+  </si>
+  <si>
+    <t>with a bigger boat, you will catch even more fish</t>
+  </si>
+  <si>
+    <t>soon you will be able another boat, hire people, and build a big business</t>
+  </si>
+  <si>
+    <t>the business was very excided</t>
+  </si>
+  <si>
+    <t>ones your business is big anough, you can sell it and make a lot of money</t>
+  </si>
+  <si>
+    <t>and what then?</t>
+  </si>
+  <si>
+    <t>и что потом?</t>
+  </si>
+  <si>
+    <t>said budinessman</t>
+  </si>
+  <si>
+    <t>then, you can retire, send time with your family, play the guitar and enjoy life with your friends - said businessman</t>
+  </si>
+  <si>
+    <t>рыбак улыбнулся и сказал</t>
+  </si>
+  <si>
+    <t>the fisherman smiled and said - is not that what I am doing right now</t>
   </si>
 </sst>
 </file>
@@ -3280,7 +3364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3340,6 +3424,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13789,8 +13886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D350"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="B297" sqref="B297"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15857,6 +15954,9 @@
       <c r="B191" s="13" t="s">
         <v>758</v>
       </c>
+      <c r="C191" s="30" t="s">
+        <v>1024</v>
+      </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="13" t="s">
@@ -15865,1086 +15965,1471 @@
       <c r="B192" s="13" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C192" s="31" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="15" t="s">
         <v>761</v>
       </c>
       <c r="B193" s="15" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C193" s="22" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
         <v>763</v>
       </c>
       <c r="B194" s="13" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C194" s="30" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="13" t="s">
         <v>765</v>
       </c>
       <c r="B195" s="13" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C195" s="31" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="15" t="s">
         <v>767</v>
       </c>
       <c r="B196" s="15" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C196" s="22" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="13" t="s">
         <v>770</v>
       </c>
       <c r="B197" s="13" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C197" s="30" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="13" t="s">
         <v>773</v>
       </c>
       <c r="B198" s="13" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C198" s="31" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="15" t="s">
         <v>774</v>
       </c>
       <c r="B199" s="15" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C199" s="22" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="13" t="s">
         <v>775</v>
       </c>
       <c r="B200" s="13" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C200" s="30" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="13" t="s">
         <v>777</v>
       </c>
       <c r="B201" s="13" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C201" s="31" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="13" t="s">
         <v>779</v>
       </c>
       <c r="B202" s="13" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C202" s="31" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="13" t="s">
         <v>781</v>
       </c>
       <c r="B203" s="13" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C203" s="31" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="15" t="s">
         <v>783</v>
       </c>
       <c r="B204" s="15" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C204" s="22" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="13" t="s">
         <v>785</v>
       </c>
       <c r="B205" s="13" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C205" s="30" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="13" t="s">
         <v>787</v>
       </c>
       <c r="B206" s="13" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C206" s="31" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="13" t="s">
         <v>789</v>
       </c>
       <c r="B207" s="13" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C207" s="31" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="13" t="s">
         <v>791</v>
       </c>
       <c r="B208" s="13" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C208" s="31" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="15" t="s">
         <v>793</v>
       </c>
       <c r="B209" s="15" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C209" s="22" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="13" t="s">
         <v>795</v>
       </c>
       <c r="B210" s="13" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C210" s="30" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="13" t="s">
         <v>798</v>
       </c>
       <c r="B211" s="13" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C211" s="31" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="13" t="s">
         <v>799</v>
       </c>
       <c r="B212" s="13" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C212" s="31" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="13" t="s">
         <v>801</v>
       </c>
       <c r="B213" s="13" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C213" s="31" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="15" t="s">
         <v>803</v>
       </c>
       <c r="B214" s="15" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C214" s="22" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="13" t="s">
         <v>805</v>
       </c>
       <c r="B215" s="13" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C215" s="30" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="15" t="s">
         <v>807</v>
       </c>
       <c r="B216" s="15" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C216" s="22" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="13" t="s">
         <v>809</v>
       </c>
       <c r="B217" s="13" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C217" s="30" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="13" t="s">
         <v>811</v>
       </c>
       <c r="B218" s="13" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C218" s="31" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="13" t="s">
         <v>813</v>
       </c>
       <c r="B219" s="13" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C219" s="31" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="15" t="s">
         <v>815</v>
       </c>
       <c r="B220" s="15" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C220" s="22" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="13" t="s">
         <v>817</v>
       </c>
       <c r="B221" s="13" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C221" s="30" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="13" t="s">
         <v>819</v>
       </c>
       <c r="B222" s="13" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C222" s="31" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="13" t="s">
         <v>821</v>
       </c>
       <c r="B223" s="13" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C223" s="31" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="13" t="s">
         <v>823</v>
       </c>
       <c r="B224" s="13" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C224" s="31" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="13" t="s">
         <v>825</v>
       </c>
       <c r="B225" s="13" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C225" s="31" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="15" t="s">
         <v>827</v>
       </c>
       <c r="B226" s="15" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C226" s="22" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="13" t="s">
         <v>829</v>
       </c>
       <c r="B227" s="13" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C227" s="27" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="13" t="s">
         <v>830</v>
       </c>
       <c r="B228" s="13" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C228" s="28" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="13" t="s">
         <v>831</v>
       </c>
       <c r="B229" s="13" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C229" s="28" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="15" t="s">
         <v>834</v>
       </c>
       <c r="B230" s="15" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C230" s="29" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="13" t="s">
         <v>836</v>
       </c>
       <c r="B231" s="13" t="s">
         <v>837</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C231" s="30" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="13" t="s">
         <v>838</v>
       </c>
       <c r="B232" s="13" t="s">
         <v>839</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C232" s="31" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="13" t="s">
         <v>840</v>
       </c>
       <c r="B233" s="13" t="s">
         <v>841</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C233" s="31" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="15" t="s">
         <v>842</v>
       </c>
       <c r="B234" s="15" t="s">
         <v>843</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C234" s="22" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="13" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B235" s="13" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C235" s="30" t="s">
         <v>844</v>
       </c>
-      <c r="B235" s="13" t="s">
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="13" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B236" s="13" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C236" s="31" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="13" t="s">
         <v>846</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="13" t="s">
+      <c r="B237" s="13" t="s">
         <v>847</v>
       </c>
-      <c r="B236" s="13" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="13" t="s">
+      <c r="C237" s="31" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="15" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B238" s="15" t="s">
         <v>848</v>
       </c>
-      <c r="B237" s="13" t="s">
+      <c r="C238" s="22" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="15" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="15" t="s">
+      <c r="B239" s="15" t="s">
         <v>850</v>
       </c>
-      <c r="B238" s="15" t="s">
+      <c r="C239" s="32" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="13" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="15" t="s">
+      <c r="B240" s="13" t="s">
         <v>852</v>
       </c>
-      <c r="B239" s="15" t="s">
+      <c r="C240" s="30" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="13" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="13" t="s">
+      <c r="B241" s="13" t="s">
         <v>854</v>
       </c>
-      <c r="B240" s="13" t="s">
+      <c r="C241" s="31" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="13" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="13" t="s">
+      <c r="B242" s="13" t="s">
         <v>856</v>
       </c>
-      <c r="B241" s="13" t="s">
+      <c r="C242" s="31" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="13" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="13" t="s">
+      <c r="B243" s="13" t="s">
         <v>858</v>
       </c>
-      <c r="B242" s="13" t="s">
+      <c r="C243" s="31" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A244" s="15" t="s">
         <v>859</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="13" t="s">
+      <c r="B244" s="15" t="s">
         <v>860</v>
       </c>
-      <c r="B243" s="13" t="s">
+      <c r="C244" s="22" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="15" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A244" s="15" t="s">
+      <c r="B245" s="15" t="s">
         <v>862</v>
       </c>
-      <c r="B244" s="15" t="s">
+      <c r="C245" s="10" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="13" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="15" t="s">
+      <c r="B246" s="13" t="s">
         <v>864</v>
       </c>
-      <c r="B245" s="15" t="s">
+      <c r="C246" s="30" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="13" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="13" t="s">
+      <c r="B247" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="B246" s="13" t="s">
+      <c r="C247" s="31" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="13" t="s">
         <v>867</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="13" t="s">
+      <c r="B248" s="13" t="s">
         <v>868</v>
       </c>
-      <c r="B247" s="13" t="s">
+      <c r="C248" s="31" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A249" s="15" t="s">
         <v>869</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="13" t="s">
+      <c r="B249" s="15" t="s">
         <v>870</v>
       </c>
-      <c r="B248" s="13" t="s">
+      <c r="C249" s="22" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="13" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A249" s="15" t="s">
+      <c r="B250" s="13" t="s">
         <v>872</v>
       </c>
-      <c r="B249" s="15" t="s">
+      <c r="C250" s="27" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="15" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="13" t="s">
+      <c r="B251" s="15" t="s">
         <v>874</v>
       </c>
-      <c r="B250" s="13" t="s">
+      <c r="C251" s="29" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="13" t="s">
+        <v>876</v>
+      </c>
+      <c r="B252" s="13" t="s">
+        <v>877</v>
+      </c>
+      <c r="C252" s="27" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="15" t="s">
         <v>875</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="15" t="s">
-        <v>876</v>
-      </c>
-      <c r="B251" s="15" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="13" t="s">
+      <c r="B253" s="15" t="s">
+        <v>878</v>
+      </c>
+      <c r="C253" s="29" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="13" t="s">
         <v>879</v>
       </c>
-      <c r="B252" s="13" t="s">
+      <c r="B254" s="13" t="s">
+        <v>886</v>
+      </c>
+      <c r="C254" s="30" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="13" t="s">
         <v>880</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="15" t="s">
-        <v>878</v>
-      </c>
-      <c r="B253" s="15" t="s">
+      <c r="B255" s="13" t="s">
+        <v>887</v>
+      </c>
+      <c r="C255" s="31" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="13" t="s">
         <v>881</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="13" t="s">
+      <c r="B256" s="13" t="s">
+        <v>888</v>
+      </c>
+      <c r="C256" s="31" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="13" t="s">
         <v>882</v>
       </c>
-      <c r="B254" s="13" t="s">
+      <c r="B257" s="13" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="13" t="s">
+      <c r="C257" s="31" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="13" t="s">
         <v>883</v>
       </c>
-      <c r="B255" s="13" t="s">
+      <c r="B258" s="13" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="13" t="s">
+      <c r="C258" s="31" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="B256" s="13" t="s">
+      <c r="B259" s="13" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="13" t="s">
+      <c r="C259" s="31" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A260" s="15" t="s">
         <v>885</v>
       </c>
-      <c r="B257" s="13" t="s">
+      <c r="B260" s="15" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="13" t="s">
-        <v>886</v>
-      </c>
-      <c r="B258" s="13" t="s">
+      <c r="C260" s="22" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" s="13" t="s">
         <v>893</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="13" t="s">
-        <v>887</v>
-      </c>
-      <c r="B259" s="13" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A260" s="15" t="s">
-        <v>888</v>
-      </c>
-      <c r="B260" s="15" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="13" t="s">
-        <v>896</v>
       </c>
       <c r="B261" s="13" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C261" s="27" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="13" t="s">
+        <v>894</v>
+      </c>
+      <c r="B262" s="13" t="s">
         <v>897</v>
       </c>
-      <c r="B262" s="13" t="s">
+      <c r="C262" s="28" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" s="13" t="s">
+        <v>895</v>
+      </c>
+      <c r="B263" s="13" t="s">
+        <v>898</v>
+      </c>
+      <c r="C263" s="28" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" s="15" t="s">
+        <v>896</v>
+      </c>
+      <c r="B264" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="C264" s="29" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" s="15" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="13" t="s">
+      <c r="B265" s="15" t="s">
+        <v>901</v>
+      </c>
+      <c r="C265" s="10" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" s="13" t="s">
+        <v>906</v>
+      </c>
+      <c r="B266" s="13" t="s">
+        <v>908</v>
+      </c>
+      <c r="C266" s="30" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" s="13" t="s">
+        <v>907</v>
+      </c>
+      <c r="B267" s="13" t="s">
+        <v>909</v>
+      </c>
+      <c r="C267" s="31" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" s="13" t="s">
+        <v>902</v>
+      </c>
+      <c r="B268" s="13" t="s">
+        <v>903</v>
+      </c>
+      <c r="C268" s="31" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" s="13" t="s">
+        <v>904</v>
+      </c>
+      <c r="B269" s="13" t="s">
+        <v>905</v>
+      </c>
+      <c r="C269" s="31" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A270" s="15" t="s">
+        <v>910</v>
+      </c>
+      <c r="B270" s="15" t="s">
+        <v>911</v>
+      </c>
+      <c r="C270" s="22" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" s="13" t="s">
+        <v>912</v>
+      </c>
+      <c r="B271" s="13" t="s">
+        <v>913</v>
+      </c>
+      <c r="C271" s="27" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="13" t="s">
+        <v>914</v>
+      </c>
+      <c r="B272" s="13" t="s">
+        <v>915</v>
+      </c>
+      <c r="C272" s="28" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="13" t="s">
+        <v>916</v>
+      </c>
+      <c r="B273" s="13" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C273" s="28" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="15" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B274" s="15" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C274" s="29" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="13" t="s">
+        <v>917</v>
+      </c>
+      <c r="B275" s="13" t="s">
+        <v>918</v>
+      </c>
+      <c r="C275" s="30" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="13" t="s">
+        <v>919</v>
+      </c>
+      <c r="B276" s="13" t="s">
+        <v>920</v>
+      </c>
+      <c r="C276" s="31" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" s="13" t="s">
+        <v>921</v>
+      </c>
+      <c r="B277" s="13" t="s">
+        <v>868</v>
+      </c>
+      <c r="C277" s="31" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A278" s="15" t="s">
+        <v>922</v>
+      </c>
+      <c r="B278" s="15" t="s">
+        <v>923</v>
+      </c>
+      <c r="C278" s="22" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" s="13" t="s">
+        <v>924</v>
+      </c>
+      <c r="B279" s="13" t="s">
+        <v>925</v>
+      </c>
+      <c r="C279" s="30" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="13" t="s">
+        <v>926</v>
+      </c>
+      <c r="B280" s="13" t="s">
+        <v>927</v>
+      </c>
+      <c r="C280" s="31" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="B281" s="13" t="s">
+        <v>929</v>
+      </c>
+      <c r="C281" s="31" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="13" t="s">
+        <v>930</v>
+      </c>
+      <c r="B282" s="13" t="s">
+        <v>931</v>
+      </c>
+      <c r="C282" s="31" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="13" t="s">
+        <v>932</v>
+      </c>
+      <c r="B283" s="13" t="s">
+        <v>933</v>
+      </c>
+      <c r="C283" s="31" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A284" s="15" t="s">
+        <v>934</v>
+      </c>
+      <c r="B284" s="15" t="s">
+        <v>935</v>
+      </c>
+      <c r="C284" s="22" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" s="15" t="s">
+        <v>936</v>
+      </c>
+      <c r="B285" s="15" t="s">
+        <v>937</v>
+      </c>
+      <c r="C285" s="10" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" s="13" t="s">
+        <v>939</v>
+      </c>
+      <c r="B286" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="C286" s="30" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" s="13" t="s">
+        <v>940</v>
+      </c>
+      <c r="B287" s="13" t="s">
+        <v>941</v>
+      </c>
+      <c r="C287" s="31" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" s="13" t="s">
+        <v>942</v>
+      </c>
+      <c r="B288" s="13" t="s">
+        <v>943</v>
+      </c>
+      <c r="C288" s="31" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" s="13" t="s">
+        <v>944</v>
+      </c>
+      <c r="B289" s="13" t="s">
+        <v>945</v>
+      </c>
+      <c r="C289" s="31" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A290" s="15" t="s">
+        <v>946</v>
+      </c>
+      <c r="B290" s="15" t="s">
+        <v>947</v>
+      </c>
+      <c r="C290" s="22" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" s="13" t="s">
+        <v>948</v>
+      </c>
+      <c r="B291" s="13" t="s">
+        <v>949</v>
+      </c>
+      <c r="C291" s="27" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="13" t="s">
+        <v>950</v>
+      </c>
+      <c r="B292" s="13" t="s">
         <v>898</v>
       </c>
-      <c r="B263" s="13" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="15" t="s">
-        <v>899</v>
-      </c>
-      <c r="B264" s="15" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="15" t="s">
-        <v>903</v>
-      </c>
-      <c r="B265" s="15" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="13" t="s">
-        <v>909</v>
-      </c>
-      <c r="B266" s="13" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="13" t="s">
-        <v>910</v>
-      </c>
-      <c r="B267" s="13" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="13" t="s">
-        <v>905</v>
-      </c>
-      <c r="B268" s="13" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="13" t="s">
-        <v>907</v>
-      </c>
-      <c r="B269" s="13" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A270" s="15" t="s">
-        <v>913</v>
-      </c>
-      <c r="B270" s="15" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="13" t="s">
-        <v>915</v>
-      </c>
-      <c r="B271" s="13" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="13" t="s">
-        <v>917</v>
-      </c>
-      <c r="B272" s="13" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="13" t="s">
-        <v>919</v>
-      </c>
-      <c r="B273" s="13" t="s">
+      <c r="C292" s="28" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="15" t="s">
+        <v>951</v>
+      </c>
+      <c r="B293" s="15" t="s">
+        <v>952</v>
+      </c>
+      <c r="C293" s="29" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="15" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B294" s="15" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C294" s="10" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" s="13" t="s">
+        <v>953</v>
+      </c>
+      <c r="B295" s="13" t="s">
+        <v>954</v>
+      </c>
+      <c r="C295" s="30" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" s="13" t="s">
+        <v>955</v>
+      </c>
+      <c r="B296" s="13" t="s">
+        <v>956</v>
+      </c>
+      <c r="C296" s="31" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" s="13" t="s">
+        <v>957</v>
+      </c>
+      <c r="B297" s="13" t="s">
+        <v>961</v>
+      </c>
+      <c r="C297" s="31" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" s="13" t="s">
+        <v>958</v>
+      </c>
+      <c r="B298" s="13" t="s">
+        <v>962</v>
+      </c>
+      <c r="C298" s="31" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" s="13" t="s">
+        <v>959</v>
+      </c>
+      <c r="B299" s="13" t="s">
+        <v>963</v>
+      </c>
+      <c r="C299" s="31" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="13" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="15" t="s">
-        <v>920</v>
-      </c>
-      <c r="B274" s="15" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="13" t="s">
-        <v>923</v>
-      </c>
-      <c r="B275" s="13" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="13" t="s">
-        <v>925</v>
-      </c>
-      <c r="B276" s="13" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="13" t="s">
-        <v>927</v>
-      </c>
-      <c r="B277" s="13" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A278" s="15" t="s">
-        <v>928</v>
-      </c>
-      <c r="B278" s="15" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="13" t="s">
-        <v>930</v>
-      </c>
-      <c r="B279" s="13" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="13" t="s">
-        <v>932</v>
-      </c>
-      <c r="B280" s="13" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="13" t="s">
-        <v>934</v>
-      </c>
-      <c r="B281" s="13" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="13" t="s">
-        <v>936</v>
-      </c>
-      <c r="B282" s="13" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="13" t="s">
-        <v>938</v>
-      </c>
-      <c r="B283" s="13" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A284" s="15" t="s">
-        <v>940</v>
-      </c>
-      <c r="B284" s="15" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="15" t="s">
-        <v>942</v>
-      </c>
-      <c r="B285" s="15" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="13" t="s">
-        <v>945</v>
-      </c>
-      <c r="B286" s="13" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="13" t="s">
-        <v>946</v>
-      </c>
-      <c r="B287" s="13" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="13" t="s">
-        <v>948</v>
-      </c>
-      <c r="B288" s="13" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="13" t="s">
-        <v>950</v>
-      </c>
-      <c r="B289" s="13" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A290" s="15" t="s">
-        <v>952</v>
-      </c>
-      <c r="B290" s="15" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="13" t="s">
-        <v>954</v>
-      </c>
-      <c r="B291" s="13" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="13" t="s">
-        <v>956</v>
-      </c>
-      <c r="B292" s="13" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="15" t="s">
-        <v>957</v>
-      </c>
-      <c r="B293" s="15" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="15" t="s">
-        <v>959</v>
-      </c>
-      <c r="B294" s="15" t="s">
+      <c r="B300" s="13" t="s">
+        <v>868</v>
+      </c>
+      <c r="C300" s="31" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A301" s="15" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="13" t="s">
-        <v>961</v>
-      </c>
-      <c r="B295" s="13" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="13" t="s">
-        <v>963</v>
-      </c>
-      <c r="B296" s="13" t="s">
+      <c r="B301" s="15" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="13" t="s">
+      <c r="C301" s="22" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" s="13" t="s">
         <v>965</v>
       </c>
-      <c r="B297" s="13" t="s">
+      <c r="B302" s="13" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C302" s="30" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" s="13" t="s">
+        <v>966</v>
+      </c>
+      <c r="B303" s="13" t="s">
+        <v>967</v>
+      </c>
+      <c r="C303" s="31" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A304" s="15" t="s">
+        <v>968</v>
+      </c>
+      <c r="B304" s="15" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="13" t="s">
-        <v>966</v>
-      </c>
-      <c r="B298" s="13" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="13" t="s">
-        <v>967</v>
-      </c>
-      <c r="B299" s="13" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="13" t="s">
-        <v>927</v>
-      </c>
-      <c r="B300" s="13" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A301" s="15" t="s">
-        <v>968</v>
-      </c>
-      <c r="B301" s="15" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="13" t="s">
-        <v>973</v>
-      </c>
-      <c r="B302" s="13" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="13" t="s">
-        <v>975</v>
-      </c>
-      <c r="B303" s="13" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A304" s="15" t="s">
-        <v>977</v>
-      </c>
-      <c r="B304" s="15" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C304" s="22" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="13"/>
       <c r="B305" s="13"/>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C305" s="26"/>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="13"/>
       <c r="B306" s="13"/>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C306" s="26"/>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="13"/>
       <c r="B307" s="13"/>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C307" s="26"/>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
       <c r="B308" s="13"/>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C308" s="26"/>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="13"/>
       <c r="B309" s="13"/>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C309" s="26"/>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="13"/>
       <c r="B310" s="13"/>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C310" s="26"/>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="13"/>
       <c r="B311" s="13"/>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C311" s="26"/>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="13"/>
       <c r="B312" s="13"/>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C312" s="26"/>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="13"/>
       <c r="B313" s="13"/>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C313" s="26"/>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="13"/>
       <c r="B314" s="13"/>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C314" s="26"/>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="13"/>
       <c r="B315" s="13"/>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C315" s="26"/>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="13"/>
       <c r="B316" s="13"/>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C316" s="26"/>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="13"/>
       <c r="B317" s="13"/>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C317" s="26"/>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
       <c r="B318" s="13"/>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C318" s="26"/>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="13"/>
       <c r="B319" s="13"/>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C319" s="26"/>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="13"/>
       <c r="B320" s="13"/>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C320" s="26"/>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="13"/>
       <c r="B321" s="13"/>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C321" s="26"/>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="13"/>
       <c r="B322" s="13"/>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C322" s="26"/>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="13"/>
       <c r="B323" s="13"/>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C323" s="26"/>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="13"/>
       <c r="B324" s="13"/>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C324" s="26"/>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
       <c r="B325" s="13"/>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C325" s="26"/>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="13"/>
       <c r="B326" s="13"/>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C326" s="26"/>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="13"/>
       <c r="B327" s="13"/>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C327" s="26"/>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="13"/>
       <c r="B328" s="13"/>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C328" s="26"/>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="13"/>
       <c r="B329" s="13"/>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C329" s="26"/>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="13"/>
       <c r="B330" s="13"/>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C330" s="26"/>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="13"/>
       <c r="B331" s="13"/>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C331" s="26"/>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="13"/>
       <c r="B332" s="13"/>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C332" s="26"/>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
       <c r="B333" s="13"/>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C333" s="26"/>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="13"/>
       <c r="B334" s="13"/>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C334" s="26"/>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="13"/>
       <c r="B335" s="13"/>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C335" s="26"/>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="13"/>
       <c r="B336" s="13"/>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C336" s="26"/>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="13"/>
       <c r="B337" s="13"/>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C337" s="26"/>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="13"/>
       <c r="B338" s="13"/>
-    </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C338" s="26"/>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="13"/>
       <c r="B339" s="13"/>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C339" s="26"/>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="13"/>
       <c r="B340" s="13"/>
-    </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C340" s="26"/>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="13"/>
       <c r="B341" s="13"/>
-    </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C341" s="26"/>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="13"/>
       <c r="B342" s="13"/>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C342" s="26"/>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="13"/>
       <c r="B343" s="13"/>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C343" s="26"/>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="13"/>
       <c r="B344" s="13"/>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C344" s="26"/>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="13"/>
       <c r="B345" s="13"/>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C345" s="26"/>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="13"/>
       <c r="B346" s="13"/>
-    </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C346" s="26"/>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="13"/>
       <c r="B347" s="13"/>
-    </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C347" s="26"/>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="13"/>
       <c r="B348" s="13"/>
-    </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C348" s="26"/>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="13"/>
       <c r="B349" s="13"/>
-    </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C349" s="26"/>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="13"/>
       <c r="B350" s="13"/>
+      <c r="C350" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16955,7 +17440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408249BA-B587-4090-9C66-27B099C0148E}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -16968,235 +17453,235 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>979</v>
+        <v>970</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>980</v>
+        <v>971</v>
       </c>
       <c r="C1" s="25"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>981</v>
+        <v>972</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>982</v>
+        <v>973</v>
       </c>
       <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>983</v>
+        <v>974</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>984</v>
+        <v>975</v>
       </c>
       <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>985</v>
+        <v>976</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>986</v>
+        <v>977</v>
       </c>
       <c r="C4" s="25"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>987</v>
+        <v>978</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>988</v>
+        <v>979</v>
       </c>
       <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>989</v>
+        <v>980</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>990</v>
+        <v>981</v>
       </c>
       <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>991</v>
+        <v>982</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>992</v>
+        <v>983</v>
       </c>
       <c r="C7" s="25"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>993</v>
+        <v>984</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>994</v>
+        <v>985</v>
       </c>
       <c r="C8" s="25"/>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>995</v>
+        <v>986</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>996</v>
+        <v>987</v>
       </c>
       <c r="C9" s="25"/>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>998</v>
+        <v>989</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="C10" s="25"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
       <c r="C11" s="25"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="C12" s="25"/>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>1003</v>
+        <v>994</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>1004</v>
+        <v>995</v>
       </c>
       <c r="C13" s="25"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>1005</v>
+        <v>996</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>1006</v>
+        <v>997</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>1007</v>
+        <v>998</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
       <c r="C15" s="25"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>1009</v>
+        <v>1000</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>1010</v>
+        <v>1001</v>
       </c>
       <c r="C16" s="25"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>1011</v>
+        <v>1002</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>1012</v>
+        <v>1003</v>
       </c>
       <c r="C17" s="25"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>1014</v>
+        <v>1005</v>
       </c>
       <c r="C18" s="25"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>1015</v>
+        <v>1006</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>1016</v>
+        <v>1007</v>
       </c>
       <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>1017</v>
+        <v>1008</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>1018</v>
+        <v>1009</v>
       </c>
       <c r="C20" s="25"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>1019</v>
+        <v>1010</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>1020</v>
+        <v>1011</v>
       </c>
       <c r="C21" s="25"/>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>1021</v>
+        <v>1012</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>1022</v>
+        <v>1013</v>
       </c>
       <c r="C22" s="25"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>1024</v>
+        <v>1015</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>1023</v>
+        <v>1014</v>
       </c>
       <c r="C23" s="25"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>1025</v>
+        <v>1016</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>1026</v>
+        <v>1017</v>
       </c>
       <c r="C24" s="25"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>1027</v>
+        <v>1018</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>1028</v>
+        <v>1019</v>
       </c>
       <c r="C25" s="25"/>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>1029</v>
+        <v>1020</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>1030</v>
+        <v>1021</v>
       </c>
       <c r="C26" s="25"/>
     </row>

</xml_diff>

<commit_message>
Add translation of technical sentences
</commit_message>
<xml_diff>
--- a/english.xlsx
+++ b/english.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popoves\Desktop\experience\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77A4024-6787-4FB1-8359-4803BAE6D664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EB2D30-79A9-473D-9B81-C70030E7DAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="words" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="1074">
   <si>
     <t>word</t>
   </si>
@@ -2955,9 +2955,6 @@
     <t>we will walk you through</t>
   </si>
   <si>
-    <t>мы проведем вас через</t>
-  </si>
-  <si>
     <t>the creation of basic poll application</t>
   </si>
   <si>
@@ -2967,15 +2964,6 @@
     <t>throughtout this tutorial, we will walk you through the creation of basic poll application</t>
   </si>
   <si>
-    <t>на протяжении всего этого руководства, мы проведем вас через срздание базового опросного приложения</t>
-  </si>
-  <si>
-    <t>it will consist if two parts</t>
-  </si>
-  <si>
-    <t>оно состоит из двух частей</t>
-  </si>
-  <si>
     <t>a public site</t>
   </si>
   <si>
@@ -3021,15 +3009,9 @@
     <t>we will assume</t>
   </si>
   <si>
-    <t>мы предполагаем</t>
-  </si>
-  <si>
     <t>we will assume you have django</t>
   </si>
   <si>
-    <t>мы предполагаем, что у вас есть django</t>
-  </si>
-  <si>
     <t>you have django installed already</t>
   </si>
   <si>
@@ -3096,48 +3078,15 @@
     <t>если django установлен, вы увидите версию вашей установки</t>
   </si>
   <si>
-    <t>the routine of local fisherman</t>
-  </si>
-  <si>
-    <t>he could not help but notice the rountine of local fisherman</t>
-  </si>
-  <si>
-    <t>an ameriacan businessman</t>
-  </si>
-  <si>
-    <t>an ameriacan businessman was on vacation in Mexico</t>
-  </si>
-  <si>
-    <t>he would fish a couple hours</t>
-  </si>
-  <si>
-    <t>he would fish a couple hours and then return home with some fish</t>
-  </si>
-  <si>
-    <t>also he would give some fish to his neighbour</t>
-  </si>
-  <si>
-    <t>the businessman noticed that in the afternoon fisherman didn’t work</t>
-  </si>
-  <si>
     <t>and enjoyed the company of his friends and neibours</t>
   </si>
   <si>
-    <t>instead, he spent time with his family, played the guitar, and enjoyed the company of his friends and neighbours</t>
-  </si>
-  <si>
     <t>the businessman approached to fisherman</t>
   </si>
   <si>
-    <t>one day, the businessman approached to fisherman and said</t>
-  </si>
-  <si>
     <t>I notcied</t>
   </si>
   <si>
-    <t>why don’t you stay out longer and catch more fish?</t>
-  </si>
-  <si>
     <t>why don’t you stays out longer and catch more fish?</t>
   </si>
   <si>
@@ -3153,33 +3102,12 @@
     <t>почему бы тебе не оставаться подольше?</t>
   </si>
   <si>
-    <t>I catch enough to support my family and little more to share with friends</t>
-  </si>
-  <si>
-    <t>I had great success building many businnes back home</t>
-  </si>
-  <si>
-    <t>first, you have to spend more time fishing, so you can catch more fish, started businessman</t>
-  </si>
-  <si>
-    <t>ok, that would be easy to do</t>
-  </si>
-  <si>
-    <t>you can then to sell extra fish and buy a bigger boat - continued businessman</t>
-  </si>
-  <si>
     <t>спросил рыбак очень вежливо</t>
   </si>
   <si>
     <t>what for? asked the fisherman very politely</t>
   </si>
   <si>
-    <t>зачем? спросил рыбак очень вежливо</t>
-  </si>
-  <si>
-    <t>with a bigger boat, you will catch even more fish</t>
-  </si>
-  <si>
     <t>soon you will be able another boat, hire people, and build a big business</t>
   </si>
   <si>
@@ -3205,6 +3133,123 @@
   </si>
   <si>
     <t>the fisherman smiled and said - is not that what I am doing right now</t>
+  </si>
+  <si>
+    <t>an american businessman</t>
+  </si>
+  <si>
+    <t>an american businessman was on vacation in Mexico</t>
+  </si>
+  <si>
+    <t>he was on beach</t>
+  </si>
+  <si>
+    <t>every day he was on beach</t>
+  </si>
+  <si>
+    <t>he could not hepl but notice</t>
+  </si>
+  <si>
+    <t>the rountine of a local fisherman</t>
+  </si>
+  <si>
+    <t>every moning</t>
+  </si>
+  <si>
+    <t>he would fish for couple of hours</t>
+  </si>
+  <si>
+    <t>instead, he spent time with his family, played the guitar and enjoyed company of his friends and neighbours</t>
+  </si>
+  <si>
+    <t>first, you have to spend more time fishing, so you can catch more fish - started businessman</t>
+  </si>
+  <si>
+    <t>для чего? спросил рыбак очень вежливо</t>
+  </si>
+  <si>
+    <t>what for? Asked the fisherman very politely</t>
+  </si>
+  <si>
+    <t>ok, that would easy to do - said fisherman</t>
+  </si>
+  <si>
+    <t>then you can sell the extra fish and buy a bigger boat - continued businessman</t>
+  </si>
+  <si>
+    <t>he would fishing for a couple of hours and then return home with some fish</t>
+  </si>
+  <si>
+    <t>also he would give some fish his neighbours</t>
+  </si>
+  <si>
+    <t>why don’t you stay out longer and to catch more fish</t>
+  </si>
+  <si>
+    <t>I catch enough to support my family, and little more to share with my friends</t>
+  </si>
+  <si>
+    <t>the businessman shook his had</t>
+  </si>
+  <si>
+    <t>I can teach you how become rich</t>
+  </si>
+  <si>
+    <t>let's learn by examle</t>
+  </si>
+  <si>
+    <t>throughout this tutorial</t>
+  </si>
+  <si>
+    <t>we will you walk through</t>
+  </si>
+  <si>
+    <t>creation of basic poll application</t>
+  </si>
+  <si>
+    <t>throughout this tutorial, we will walk you through creation of basic poll application</t>
+  </si>
+  <si>
+    <t>оно будет состоять из двух частей</t>
+  </si>
+  <si>
+    <t>it will consist of two parts</t>
+  </si>
+  <si>
+    <t>it will cosist of two parts</t>
+  </si>
+  <si>
+    <t>an admin site</t>
+  </si>
+  <si>
+    <t>that lets you add, change and delete polls</t>
+  </si>
+  <si>
+    <t>мы будем предполагать</t>
+  </si>
+  <si>
+    <t>мы будем вести вас через</t>
+  </si>
+  <si>
+    <t>на протяжении всего этого руководства, мы будем вести вас через создание базового опросного приложения</t>
+  </si>
+  <si>
+    <t>мы будем предполагать, что у вас есть django</t>
+  </si>
+  <si>
+    <t>we will assume that you have Django installed already</t>
+  </si>
+  <si>
+    <t>we will assume that you have Django</t>
+  </si>
+  <si>
+    <t>you have Django installed already</t>
+  </si>
+  <si>
+    <t>you can tell djang is installed</t>
+  </si>
+  <si>
+    <t>if dajngo is installed</t>
   </si>
 </sst>
 </file>
@@ -3287,7 +3332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -3360,11 +3405,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3437,6 +3513,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13886,8 +13971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C311" sqref="C311"/>
+    <sheetView topLeftCell="A286" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15955,7 +16040,7 @@
         <v>758</v>
       </c>
       <c r="C191" s="30" t="s">
-        <v>1024</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -15977,7 +16062,7 @@
         <v>762</v>
       </c>
       <c r="C193" s="22" t="s">
-        <v>1025</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -15999,7 +16084,7 @@
         <v>766</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>765</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -16010,7 +16095,7 @@
         <v>768</v>
       </c>
       <c r="C196" s="22" t="s">
-        <v>767</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -16021,7 +16106,7 @@
         <v>769</v>
       </c>
       <c r="C197" s="30" t="s">
-        <v>770</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -16032,7 +16117,7 @@
         <v>771</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>1022</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -16043,7 +16128,7 @@
         <v>772</v>
       </c>
       <c r="C199" s="22" t="s">
-        <v>1023</v>
+        <v>774</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -16054,7 +16139,7 @@
         <v>776</v>
       </c>
       <c r="C200" s="30" t="s">
-        <v>775</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -16120,7 +16205,7 @@
         <v>788</v>
       </c>
       <c r="C206" s="31" t="s">
-        <v>1026</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -16153,7 +16238,7 @@
         <v>794</v>
       </c>
       <c r="C209" s="22" t="s">
-        <v>1027</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -16230,7 +16315,7 @@
         <v>808</v>
       </c>
       <c r="C216" s="22" t="s">
-        <v>1028</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -16274,7 +16359,7 @@
         <v>816</v>
       </c>
       <c r="C220" s="22" t="s">
-        <v>1029</v>
+        <v>815</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -16329,7 +16414,7 @@
         <v>826</v>
       </c>
       <c r="C225" s="31" t="s">
-        <v>1030</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -16340,7 +16425,7 @@
         <v>828</v>
       </c>
       <c r="C226" s="22" t="s">
-        <v>1031</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -16362,7 +16447,7 @@
         <v>832</v>
       </c>
       <c r="C228" s="28" t="s">
-        <v>1032</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -16384,7 +16469,7 @@
         <v>835</v>
       </c>
       <c r="C230" s="29" t="s">
-        <v>1033</v>
+        <v>834</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -16406,7 +16491,7 @@
         <v>839</v>
       </c>
       <c r="C232" s="31" t="s">
-        <v>1034</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -16433,10 +16518,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="13" t="s">
-        <v>1038</v>
+        <v>1021</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>1039</v>
+        <v>1022</v>
       </c>
       <c r="C235" s="30" t="s">
         <v>844</v>
@@ -16444,10 +16529,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="13" t="s">
-        <v>1037</v>
+        <v>1020</v>
       </c>
       <c r="B236" s="13" t="s">
-        <v>1040</v>
+        <v>1023</v>
       </c>
       <c r="C236" s="31" t="s">
         <v>845</v>
@@ -16466,13 +16551,13 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="15" t="s">
-        <v>1036</v>
+        <v>1019</v>
       </c>
       <c r="B238" s="15" t="s">
         <v>848</v>
       </c>
       <c r="C238" s="22" t="s">
-        <v>1035</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -16538,7 +16623,7 @@
         <v>860</v>
       </c>
       <c r="C244" s="22" t="s">
-        <v>1041</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -16549,7 +16634,7 @@
         <v>862</v>
       </c>
       <c r="C245" s="10" t="s">
-        <v>861</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -16593,7 +16678,7 @@
         <v>870</v>
       </c>
       <c r="C249" s="22" t="s">
-        <v>1042</v>
+        <v>869</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -16615,7 +16700,7 @@
         <v>874</v>
       </c>
       <c r="C251" s="29" t="s">
-        <v>873</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -16714,7 +16799,7 @@
         <v>892</v>
       </c>
       <c r="C260" s="22" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -16758,7 +16843,7 @@
         <v>899</v>
       </c>
       <c r="C264" s="29" t="s">
-        <v>1044</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -16824,7 +16909,7 @@
         <v>911</v>
       </c>
       <c r="C270" s="22" t="s">
-        <v>1045</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -16854,7 +16939,7 @@
         <v>916</v>
       </c>
       <c r="B273" s="13" t="s">
-        <v>1046</v>
+        <v>1024</v>
       </c>
       <c r="C273" s="28" t="s">
         <v>916</v>
@@ -16862,13 +16947,13 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="15" t="s">
-        <v>1047</v>
+        <v>1025</v>
       </c>
       <c r="B274" s="15" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="C274" s="29" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -16912,7 +16997,7 @@
         <v>923</v>
       </c>
       <c r="C278" s="22" t="s">
-        <v>1049</v>
+        <v>922</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -16978,7 +17063,7 @@
         <v>935</v>
       </c>
       <c r="C284" s="22" t="s">
-        <v>1050</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -16989,7 +17074,7 @@
         <v>937</v>
       </c>
       <c r="C285" s="10" t="s">
-        <v>1051</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -17044,7 +17129,7 @@
         <v>947</v>
       </c>
       <c r="C290" s="22" t="s">
-        <v>1052</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -17082,13 +17167,13 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="15" t="s">
-        <v>1053</v>
+        <v>1029</v>
       </c>
       <c r="B294" s="15" t="s">
-        <v>1054</v>
+        <v>1030</v>
       </c>
       <c r="C294" s="10" t="s">
-        <v>1053</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -17154,7 +17239,7 @@
         <v>868</v>
       </c>
       <c r="C300" s="31" t="s">
-        <v>1055</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -17165,7 +17250,7 @@
         <v>964</v>
       </c>
       <c r="C301" s="22" t="s">
-        <v>1056</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -17173,7 +17258,7 @@
         <v>965</v>
       </c>
       <c r="B302" s="13" t="s">
-        <v>1057</v>
+        <v>1033</v>
       </c>
       <c r="C302" s="30" t="s">
         <v>965</v>
@@ -17198,7 +17283,7 @@
         <v>969</v>
       </c>
       <c r="C304" s="22" t="s">
-        <v>1058</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -17440,8 +17525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408249BA-B587-4090-9C66-27B099C0148E}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17458,7 +17543,9 @@
       <c r="B1" s="15" t="s">
         <v>971</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="32" t="s">
+        <v>1055</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -17467,223 +17554,273 @@
       <c r="B2" s="13" t="s">
         <v>973</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="30" t="s">
+        <v>1056</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>974</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>975</v>
-      </c>
-      <c r="C3" s="25"/>
+        <v>1066</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>1057</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>975</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>976</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>977</v>
-      </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="31" t="s">
+        <v>1058</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>979</v>
-      </c>
-      <c r="C5" s="25"/>
+        <v>1067</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>1059</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>980</v>
+        <v>1061</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>981</v>
-      </c>
-      <c r="C6" s="25"/>
+        <v>1060</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>1062</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>983</v>
-      </c>
-      <c r="C7" s="25"/>
+        <v>979</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>985</v>
-      </c>
-      <c r="C8" s="25"/>
+        <v>981</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>980</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>987</v>
-      </c>
-      <c r="C9" s="25"/>
+        <v>983</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>982</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>988</v>
-      </c>
-      <c r="C10" s="25"/>
+        <v>984</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>985</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>991</v>
-      </c>
-      <c r="C11" s="25"/>
+        <v>987</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>1063</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>993</v>
-      </c>
-      <c r="C12" s="25"/>
+        <v>989</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>1064</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>995</v>
-      </c>
-      <c r="C13" s="25"/>
+        <v>991</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>990</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>997</v>
-      </c>
-      <c r="C14" s="25"/>
+        <v>1065</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>992</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>998</v>
+        <v>993</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>999</v>
-      </c>
-      <c r="C15" s="25"/>
+        <v>1068</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>1070</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>1000</v>
+        <v>994</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C16" s="25"/>
+        <v>995</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>1071</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C17" s="25"/>
+        <v>997</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>1069</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C18" s="25"/>
+        <v>999</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>998</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C19" s="25"/>
+        <v>1001</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>1072</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>1009</v>
-      </c>
-      <c r="C20" s="25"/>
+        <v>1003</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>1002</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C21" s="25"/>
+        <v>1005</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>1004</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C22" s="25"/>
+        <v>1007</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>1006</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>1014</v>
-      </c>
-      <c r="C23" s="25"/>
+        <v>1008</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>1073</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>1017</v>
-      </c>
-      <c r="C24" s="25"/>
+        <v>1011</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C25" s="25"/>
+        <v>1013</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>1012</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>1021</v>
-      </c>
-      <c r="C26" s="25"/>
+        <v>1015</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>1014</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>

</xml_diff>

<commit_message>
Add Weekends with my grandkids story
</commit_message>
<xml_diff>
--- a/english.xlsx
+++ b/english.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popoves\Desktop\experience\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DDD8F8-B6C9-41A2-B070-A500B2A55FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855D4AE6-55DA-4296-9947-307CB5A4B403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="1054">
   <si>
     <t>word</t>
   </si>
@@ -2806,9 +2806,6 @@
     <t>да, просто пройдите прямо по этому коридору и поверните на лево</t>
   </si>
   <si>
-    <t>you'll see sings</t>
-  </si>
-  <si>
     <t>вы увидите указатели</t>
   </si>
   <si>
@@ -2869,12 +2866,6 @@
     <t>hello ma'am</t>
   </si>
   <si>
-    <t>of course, may I see your passport please?</t>
-  </si>
-  <si>
-    <t>alright, your bag will be transferred automatically in Amsterdam</t>
-  </si>
-  <si>
     <t>where security is?</t>
   </si>
   <si>
@@ -2926,42 +2917,12 @@
     <t>ваша сумка будет</t>
   </si>
   <si>
-    <t>hi, i need to check in for my flight to new york</t>
-  </si>
-  <si>
-    <t>thank you, are you checking in any luggage today?</t>
-  </si>
-  <si>
     <t>great, could you please place it on the scale?</t>
   </si>
   <si>
     <t>sure, here you go</t>
   </si>
   <si>
-    <t>your bags is within weight limit</t>
-  </si>
-  <si>
-    <t>thank you, your bag is withing weight limit</t>
-  </si>
-  <si>
-    <t>your bag will be trasferred automatically in Amsterdam</t>
-  </si>
-  <si>
-    <t>that is not problem</t>
-  </si>
-  <si>
-    <t>or any special reuests for your flight?</t>
-  </si>
-  <si>
-    <t>do you have any items that need to declare or any special requests for your flight?</t>
-  </si>
-  <si>
-    <t>yes, just head straight down this hall and turn left</t>
-  </si>
-  <si>
-    <t>you'll see sings for the security checkpoint</t>
-  </si>
-  <si>
     <t>do you have any items that need to be declaerd?</t>
   </si>
   <si>
@@ -2971,16 +2932,298 @@
     <t>thanks a lot for you help</t>
   </si>
   <si>
-    <t>thaks a lot for your help</t>
-  </si>
-  <si>
     <t>have a safe trip</t>
   </si>
   <si>
-    <t>счастливого пути</t>
-  </si>
-  <si>
     <t>repeat</t>
+  </si>
+  <si>
+    <t>hi, I need to check in for my flight to new york</t>
+  </si>
+  <si>
+    <t>of course, may I see your passport?</t>
+  </si>
+  <si>
+    <t>thank you, are you check in any luggage today?</t>
+  </si>
+  <si>
+    <t>thank you, your bag is within weight limit</t>
+  </si>
+  <si>
+    <t>alright, your bag will be transferred automatically in Amstedam</t>
+  </si>
+  <si>
+    <t>that is not a problem</t>
+  </si>
+  <si>
+    <t>do you have any items that need to be declared, or any special requests for you flight?</t>
+  </si>
+  <si>
+    <t>okey, here are you boarding passes</t>
+  </si>
+  <si>
+    <t>just head straight down the hall</t>
+  </si>
+  <si>
+    <t>yes, just head straight down the hall and turn left</t>
+  </si>
+  <si>
+    <t>you'll see signs</t>
+  </si>
+  <si>
+    <t>you'll see signs for the security checkpoint</t>
+  </si>
+  <si>
+    <t>thanks a lot for your help</t>
+  </si>
+  <si>
+    <t>безопастного пути</t>
+  </si>
+  <si>
+    <t>weekends with my grandkids</t>
+  </si>
+  <si>
+    <t>выходные с моими внуками</t>
+  </si>
+  <si>
+    <t>my name is Rick</t>
+  </si>
+  <si>
+    <t>меня зовут Рик</t>
+  </si>
+  <si>
+    <t>I live with my wife, Susan</t>
+  </si>
+  <si>
+    <t>я живу со своей женой, Сюзан</t>
+  </si>
+  <si>
+    <t>we live in a small house</t>
+  </si>
+  <si>
+    <t>but we have a big garden</t>
+  </si>
+  <si>
+    <t>we live in a small house, but we have a big garden</t>
+  </si>
+  <si>
+    <t>мы живем в маленьком доме</t>
+  </si>
+  <si>
+    <t>но у нас есть большой сад</t>
+  </si>
+  <si>
+    <t>мы живем в маленьком доме, но у нас есть большой сад</t>
+  </si>
+  <si>
+    <t>we are both retired</t>
+  </si>
+  <si>
+    <t>so we have a lot of free time</t>
+  </si>
+  <si>
+    <t>we are both retired so we have a lot of free time</t>
+  </si>
+  <si>
+    <t>мы оба на пенсии</t>
+  </si>
+  <si>
+    <t>поэтому у нас много свободного времени</t>
+  </si>
+  <si>
+    <t>мы оба на пенсии, поэтому у нас много свободного времени</t>
+  </si>
+  <si>
+    <t>we love spending time in out garden</t>
+  </si>
+  <si>
+    <t>мы любим проводить время в нашем саду</t>
+  </si>
+  <si>
+    <t>my wife takes care of the flowers</t>
+  </si>
+  <si>
+    <t>моя жена ухаживает за растениями</t>
+  </si>
+  <si>
+    <t>I take care of the fruits and vegetables</t>
+  </si>
+  <si>
+    <t>я забочусь о фруктах и овощях</t>
+  </si>
+  <si>
+    <t>our grandchildren, Mia and Jake</t>
+  </si>
+  <si>
+    <t>come to visit us every weekend</t>
+  </si>
+  <si>
+    <t>our grandchildren, Mia and Jake, come to visit us every weekend</t>
+  </si>
+  <si>
+    <t>наши внуки, Мия и Джейк</t>
+  </si>
+  <si>
+    <t>приезжают к нам каждые выходные</t>
+  </si>
+  <si>
+    <t>наши внуки, Мия и Джейк, приезжают к нам каждые выходные</t>
+  </si>
+  <si>
+    <t>we are always so happy to see them</t>
+  </si>
+  <si>
+    <t>мы всегда так рады их видеть</t>
+  </si>
+  <si>
+    <t>they love to spend time in the garden</t>
+  </si>
+  <si>
+    <t>они любят проводить время в саду</t>
+  </si>
+  <si>
+    <t>they love to see the plants grow every week</t>
+  </si>
+  <si>
+    <t>им нравиться наблюдать за тем, как растения растут каждые выходные</t>
+  </si>
+  <si>
+    <t>I teach them how to plant and grow vegetables</t>
+  </si>
+  <si>
+    <t>я учу их, как сажать и выращивать овощи</t>
+  </si>
+  <si>
+    <t>they water the plants and pick raspberries and tomatoes</t>
+  </si>
+  <si>
+    <t>они поливают растения и собирают малину и помидоры</t>
+  </si>
+  <si>
+    <t>they taste so good</t>
+  </si>
+  <si>
+    <t>они такие вкусные</t>
+  </si>
+  <si>
+    <t>in the evenings after dinner</t>
+  </si>
+  <si>
+    <t>we sit in the living room and talk</t>
+  </si>
+  <si>
+    <t>in the evening after dinner, we sit in living room and talk</t>
+  </si>
+  <si>
+    <t>по вечерам после ужина</t>
+  </si>
+  <si>
+    <t>мы сидим в гостинной и разговариваем</t>
+  </si>
+  <si>
+    <t>по вечерам после ужина мы сидим в гостинной и разговариваем</t>
+  </si>
+  <si>
+    <t>Mia and Jake ask me about my life</t>
+  </si>
+  <si>
+    <t>Миа и Джейк спрашивают меня о моей жизни</t>
+  </si>
+  <si>
+    <t>I talk about when I was their age</t>
+  </si>
+  <si>
+    <t>я рассказываю о том, когда я был в их возрасте</t>
+  </si>
+  <si>
+    <t>I tell them how I got into trouble</t>
+  </si>
+  <si>
+    <t>я рассказываю им, как я попадал в неприятности</t>
+  </si>
+  <si>
+    <t>Mia and Jake listen and laugh</t>
+  </si>
+  <si>
+    <t>Мия и Джейк слушают и смеются</t>
+  </si>
+  <si>
+    <t>Susan bakes cookies for dessert</t>
+  </si>
+  <si>
+    <t>Сюзан печет печенье на десерт</t>
+  </si>
+  <si>
+    <t>Mia and Jake eat the cookies with milk</t>
+  </si>
+  <si>
+    <t>Мия и Джейк едят печенье с молоком</t>
+  </si>
+  <si>
+    <t>they love grandma's baking</t>
+  </si>
+  <si>
+    <t>we are a little sad</t>
+  </si>
+  <si>
+    <t>нам немного грустно</t>
+  </si>
+  <si>
+    <t>они любят бабушкину выпечку</t>
+  </si>
+  <si>
+    <t>when it is time for the kids to go home</t>
+  </si>
+  <si>
+    <t>когда детям пора идти домой</t>
+  </si>
+  <si>
+    <t>we are a little sad, when it is time for the kids to go home</t>
+  </si>
+  <si>
+    <t>нам немного грустно, когда детям пора идти домой</t>
+  </si>
+  <si>
+    <t>Mia and Jake are sad too</t>
+  </si>
+  <si>
+    <t>Мия и Джейк тоже грустят</t>
+  </si>
+  <si>
+    <t>but weare happy to know</t>
+  </si>
+  <si>
+    <t>но вы рады знать</t>
+  </si>
+  <si>
+    <t>they will come again next week</t>
+  </si>
+  <si>
+    <t>они придут снова на следующей неделе</t>
+  </si>
+  <si>
+    <t>but we are happy to know they will come again next week</t>
+  </si>
+  <si>
+    <t>но мы рады знать, что они придут снова на следующей неделе</t>
+  </si>
+  <si>
+    <t>we always look forward</t>
+  </si>
+  <si>
+    <t>to their next visit</t>
+  </si>
+  <si>
+    <t>we always look forward to their next visit</t>
+  </si>
+  <si>
+    <t>мы всегда с нетерпением ждем</t>
+  </si>
+  <si>
+    <t>их следующего визита</t>
+  </si>
+  <si>
+    <t>мы всегда с нетерпением ждем их следующего визита</t>
   </si>
 </sst>
 </file>
@@ -13713,10 +13956,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D267"/>
+  <dimension ref="A1:D368"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B299" sqref="B299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13737,7 +13980,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>972</v>
+        <v>957</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -16103,7 +16346,7 @@
         <v>900</v>
       </c>
       <c r="C217" s="29" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -16125,7 +16368,7 @@
         <v>866</v>
       </c>
       <c r="C219" s="29" t="s">
-        <v>954</v>
+        <v>958</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -16136,7 +16379,7 @@
         <v>867</v>
       </c>
       <c r="C220" s="29" t="s">
-        <v>935</v>
+        <v>959</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -16158,7 +16401,7 @@
         <v>902</v>
       </c>
       <c r="C222" s="29" t="s">
-        <v>955</v>
+        <v>960</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -16180,7 +16423,7 @@
         <v>875</v>
       </c>
       <c r="C224" s="29" t="s">
-        <v>956</v>
+        <v>951</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -16191,7 +16434,7 @@
         <v>877</v>
       </c>
       <c r="C225" s="29" t="s">
-        <v>957</v>
+        <v>952</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -16207,24 +16450,24 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="10" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="B227" s="10" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="C227" s="29" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="10" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="B228" s="10" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="C228" s="29" t="s">
-        <v>958</v>
+        <v>943</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -16235,40 +16478,40 @@
         <v>879</v>
       </c>
       <c r="C229" s="29" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="10" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="B230" s="10" t="s">
         <v>249</v>
       </c>
       <c r="C230" s="29" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="10" t="s">
+        <v>947</v>
+      </c>
+      <c r="B231" s="10" t="s">
         <v>950</v>
       </c>
-      <c r="B231" s="10" t="s">
-        <v>953</v>
-      </c>
       <c r="C231" s="29" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="10" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="B232" s="10" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="C232" s="29" t="s">
-        <v>960</v>
+        <v>948</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -16279,7 +16522,7 @@
         <v>903</v>
       </c>
       <c r="C233" s="29" t="s">
-        <v>936</v>
+        <v>962</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -16312,18 +16555,18 @@
         <v>886</v>
       </c>
       <c r="C236" s="29" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="10" t="s">
-        <v>966</v>
+        <v>953</v>
       </c>
       <c r="B237" s="10" t="s">
         <v>890</v>
       </c>
       <c r="C237" s="27" t="s">
-        <v>967</v>
+        <v>954</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -16334,7 +16577,7 @@
         <v>889</v>
       </c>
       <c r="C238" s="28" t="s">
-        <v>962</v>
+        <v>888</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -16345,7 +16588,7 @@
         <v>891</v>
       </c>
       <c r="C239" s="19" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -16367,7 +16610,7 @@
         <v>895</v>
       </c>
       <c r="C241" s="29" t="s">
-        <v>894</v>
+        <v>965</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -16375,7 +16618,7 @@
         <v>896</v>
       </c>
       <c r="B242" s="12" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="C242" s="29" t="s">
         <v>896</v>
@@ -16394,24 +16637,24 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="10" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="B244" s="14" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="C244" s="27" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="10" t="s">
+        <v>934</v>
+      </c>
+      <c r="B245" s="14" t="s">
         <v>937</v>
       </c>
-      <c r="B245" s="14" t="s">
-        <v>940</v>
-      </c>
       <c r="C245" s="28" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -16444,7 +16687,7 @@
         <v>909</v>
       </c>
       <c r="C248" s="25" t="s">
-        <v>908</v>
+        <v>966</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -16466,129 +16709,799 @@
         <v>913</v>
       </c>
       <c r="C250" s="26" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="10" t="s">
+        <v>968</v>
+      </c>
+      <c r="B251" s="10" t="s">
         <v>914</v>
       </c>
-      <c r="B251" s="10" t="s">
-        <v>915</v>
-      </c>
       <c r="C251" s="24" t="s">
-        <v>914</v>
+        <v>968</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="10" t="s">
+        <v>938</v>
+      </c>
+      <c r="B252" s="10" t="s">
+        <v>939</v>
+      </c>
+      <c r="C252" s="25" t="s">
         <v>941</v>
-      </c>
-      <c r="B252" s="10" t="s">
-        <v>942</v>
-      </c>
-      <c r="C252" s="25" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
+        <v>915</v>
+      </c>
+      <c r="B253" s="12" t="s">
         <v>916</v>
       </c>
-      <c r="B253" s="12" t="s">
-        <v>917</v>
-      </c>
       <c r="C253" s="26" t="s">
-        <v>965</v>
+        <v>969</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="12" t="s">
-        <v>968</v>
+        <v>955</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C254" s="8" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
+        <v>918</v>
+      </c>
+      <c r="B255" s="12" t="s">
         <v>919</v>
       </c>
-      <c r="B255" s="12" t="s">
-        <v>920</v>
-      </c>
       <c r="C255" s="8" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="12" t="s">
-        <v>970</v>
+        <v>956</v>
       </c>
       <c r="B256" s="12" t="s">
         <v>971</v>
       </c>
       <c r="C256" s="8" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" s="10"/>
-      <c r="B257" s="10"/>
-      <c r="C257" s="23"/>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" s="10"/>
-      <c r="B258" s="10"/>
+        <v>956</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="21"/>
+      <c r="B257" s="21"/>
+      <c r="C257" s="9"/>
+      <c r="D257" s="9"/>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="10" t="s">
+        <v>972</v>
+      </c>
+      <c r="B258" s="10" t="s">
+        <v>973</v>
+      </c>
       <c r="C258" s="23"/>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="10"/>
-      <c r="B259" s="10"/>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="10" t="s">
+        <v>974</v>
+      </c>
+      <c r="B259" s="10" t="s">
+        <v>975</v>
+      </c>
       <c r="C259" s="23"/>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="10"/>
-      <c r="B260" s="10"/>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="10" t="s">
+        <v>976</v>
+      </c>
+      <c r="B260" s="10" t="s">
+        <v>977</v>
+      </c>
       <c r="C260" s="23"/>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261" s="10"/>
-      <c r="B261" s="10"/>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="12" t="s">
+        <v>978</v>
+      </c>
+      <c r="B261" s="12" t="s">
+        <v>981</v>
+      </c>
       <c r="C261" s="23"/>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" s="10"/>
-      <c r="B262" s="10"/>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="12" t="s">
+        <v>979</v>
+      </c>
+      <c r="B262" s="12" t="s">
+        <v>982</v>
+      </c>
       <c r="C262" s="23"/>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" s="10"/>
-      <c r="B263" s="10"/>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="10" t="s">
+        <v>980</v>
+      </c>
+      <c r="B263" s="10" t="s">
+        <v>983</v>
+      </c>
       <c r="C263" s="23"/>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" s="10"/>
-      <c r="B264" s="10"/>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="12" t="s">
+        <v>984</v>
+      </c>
+      <c r="B264" s="12" t="s">
+        <v>987</v>
+      </c>
       <c r="C264" s="23"/>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A265" s="10"/>
-      <c r="B265" s="10"/>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="12" t="s">
+        <v>985</v>
+      </c>
+      <c r="B265" s="12" t="s">
+        <v>988</v>
+      </c>
       <c r="C265" s="23"/>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A266" s="10"/>
-      <c r="B266" s="10"/>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="10" t="s">
+        <v>986</v>
+      </c>
+      <c r="B266" s="10" t="s">
+        <v>989</v>
+      </c>
       <c r="C266" s="23"/>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A267" s="10"/>
-      <c r="B267" s="10"/>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="10" t="s">
+        <v>990</v>
+      </c>
+      <c r="B267" s="10" t="s">
+        <v>991</v>
+      </c>
       <c r="C267" s="23"/>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="10" t="s">
+        <v>992</v>
+      </c>
+      <c r="B268" s="10" t="s">
+        <v>993</v>
+      </c>
+      <c r="C268" s="23"/>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" s="10" t="s">
+        <v>994</v>
+      </c>
+      <c r="B269" s="10" t="s">
+        <v>995</v>
+      </c>
+      <c r="C269" s="23"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="B270" s="12" t="s">
+        <v>999</v>
+      </c>
+      <c r="C270" s="23"/>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="12" t="s">
+        <v>997</v>
+      </c>
+      <c r="B271" s="12" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C271" s="23"/>
+    </row>
+    <row r="272" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A272" s="10" t="s">
+        <v>998</v>
+      </c>
+      <c r="B272" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C272" s="23"/>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="10" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B273" s="10" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C273" s="23"/>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="10" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B274" s="10" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C274" s="23"/>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="10" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B275" s="10" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C275" s="23"/>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="10" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B276" s="10" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C276" s="23"/>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" s="10" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B277" s="10" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C277" s="23"/>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B278" s="10" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C278" s="23"/>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" s="12" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B279" s="12" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C279" s="23"/>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="12" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B280" s="12" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C280" s="23"/>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="10" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B281" s="10" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C281" s="23"/>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="10" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B282" s="10" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C282" s="23"/>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="10" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B283" s="10" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C283" s="23"/>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" s="10" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B284" s="10" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C284" s="23"/>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" s="10" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B285" s="10" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C285" s="23"/>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" s="10" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B286" s="10" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C286" s="23"/>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" s="10" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B287" s="10" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C287" s="23"/>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" s="10" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B288" s="10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C288" s="23"/>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" s="12" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B289" s="12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C289" s="23"/>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" s="12" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B290" s="12" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C290" s="23"/>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" s="10" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B291" s="10" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C291" s="23"/>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="10" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B292" s="10" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C292" s="23"/>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="12" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B293" s="12" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C293" s="23"/>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="12" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B294" s="12" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C294" s="23"/>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" s="10" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B295" s="10" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C295" s="23"/>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" s="10" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B296" s="10" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C296" s="23"/>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" s="10" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B297" s="10" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C297" s="23"/>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" s="10" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B298" s="10" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C298" s="23"/>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" s="10"/>
+      <c r="B299" s="10"/>
+      <c r="C299" s="23"/>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="10"/>
+      <c r="B300" s="10"/>
+      <c r="C300" s="23"/>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" s="10"/>
+      <c r="B301" s="10"/>
+      <c r="C301" s="23"/>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" s="10"/>
+      <c r="B302" s="10"/>
+      <c r="C302" s="23"/>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" s="10"/>
+      <c r="B303" s="10"/>
+      <c r="C303" s="23"/>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" s="10"/>
+      <c r="B304" s="10"/>
+      <c r="C304" s="23"/>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" s="10"/>
+      <c r="B305" s="10"/>
+      <c r="C305" s="23"/>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" s="10"/>
+      <c r="B306" s="10"/>
+      <c r="C306" s="23"/>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" s="10"/>
+      <c r="B307" s="10"/>
+      <c r="C307" s="23"/>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" s="10"/>
+      <c r="B308" s="10"/>
+      <c r="C308" s="23"/>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" s="10"/>
+      <c r="B309" s="10"/>
+      <c r="C309" s="23"/>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" s="10"/>
+      <c r="B310" s="10"/>
+      <c r="C310" s="23"/>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" s="10"/>
+      <c r="B311" s="10"/>
+      <c r="C311" s="23"/>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" s="10"/>
+      <c r="B312" s="10"/>
+      <c r="C312" s="23"/>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" s="10"/>
+      <c r="B313" s="10"/>
+      <c r="C313" s="23"/>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" s="10"/>
+      <c r="B314" s="10"/>
+      <c r="C314" s="23"/>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" s="10"/>
+      <c r="B315" s="10"/>
+      <c r="C315" s="23"/>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" s="10"/>
+      <c r="B316" s="10"/>
+      <c r="C316" s="23"/>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" s="10"/>
+      <c r="B317" s="10"/>
+      <c r="C317" s="23"/>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" s="10"/>
+      <c r="B318" s="10"/>
+      <c r="C318" s="23"/>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" s="10"/>
+      <c r="B319" s="10"/>
+      <c r="C319" s="23"/>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" s="10"/>
+      <c r="B320" s="10"/>
+      <c r="C320" s="23"/>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" s="10"/>
+      <c r="B321" s="10"/>
+      <c r="C321" s="23"/>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" s="10"/>
+      <c r="B322" s="10"/>
+      <c r="C322" s="23"/>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" s="10"/>
+      <c r="B323" s="10"/>
+      <c r="C323" s="23"/>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" s="10"/>
+      <c r="B324" s="10"/>
+      <c r="C324" s="23"/>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" s="10"/>
+      <c r="B325" s="10"/>
+      <c r="C325" s="23"/>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" s="10"/>
+      <c r="B326" s="10"/>
+      <c r="C326" s="23"/>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" s="10"/>
+      <c r="B327" s="10"/>
+      <c r="C327" s="23"/>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" s="10"/>
+      <c r="B328" s="10"/>
+      <c r="C328" s="23"/>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" s="10"/>
+      <c r="B329" s="10"/>
+      <c r="C329" s="23"/>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" s="10"/>
+      <c r="B330" s="10"/>
+      <c r="C330" s="23"/>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" s="10"/>
+      <c r="B331" s="10"/>
+      <c r="C331" s="23"/>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" s="10"/>
+      <c r="B332" s="10"/>
+      <c r="C332" s="23"/>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" s="10"/>
+      <c r="B333" s="10"/>
+      <c r="C333" s="23"/>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" s="10"/>
+      <c r="B334" s="10"/>
+      <c r="C334" s="23"/>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" s="10"/>
+      <c r="B335" s="10"/>
+      <c r="C335" s="23"/>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" s="10"/>
+      <c r="B336" s="10"/>
+      <c r="C336" s="23"/>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" s="10"/>
+      <c r="B337" s="10"/>
+      <c r="C337" s="23"/>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" s="10"/>
+      <c r="B338" s="10"/>
+      <c r="C338" s="23"/>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" s="10"/>
+      <c r="B339" s="10"/>
+      <c r="C339" s="23"/>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" s="10"/>
+      <c r="B340" s="10"/>
+      <c r="C340" s="23"/>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" s="10"/>
+      <c r="B341" s="10"/>
+      <c r="C341" s="23"/>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342" s="10"/>
+      <c r="B342" s="10"/>
+      <c r="C342" s="23"/>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" s="10"/>
+      <c r="B343" s="10"/>
+      <c r="C343" s="23"/>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" s="10"/>
+      <c r="B344" s="10"/>
+      <c r="C344" s="23"/>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" s="10"/>
+      <c r="B345" s="10"/>
+      <c r="C345" s="23"/>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" s="10"/>
+      <c r="B346" s="10"/>
+      <c r="C346" s="23"/>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" s="10"/>
+      <c r="B347" s="10"/>
+      <c r="C347" s="23"/>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348" s="10"/>
+      <c r="B348" s="10"/>
+      <c r="C348" s="23"/>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" s="10"/>
+      <c r="B349" s="10"/>
+      <c r="C349" s="23"/>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" s="10"/>
+      <c r="B350" s="10"/>
+      <c r="C350" s="23"/>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" s="10"/>
+      <c r="B351" s="10"/>
+      <c r="C351" s="23"/>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352" s="10"/>
+      <c r="B352" s="10"/>
+      <c r="C352" s="23"/>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" s="10"/>
+      <c r="B353" s="10"/>
+      <c r="C353" s="23"/>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" s="10"/>
+      <c r="B354" s="10"/>
+      <c r="C354" s="23"/>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" s="10"/>
+      <c r="B355" s="10"/>
+      <c r="C355" s="23"/>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" s="10"/>
+      <c r="B356" s="10"/>
+      <c r="C356" s="23"/>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" s="10"/>
+      <c r="B357" s="10"/>
+      <c r="C357" s="23"/>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" s="10"/>
+      <c r="B358" s="10"/>
+      <c r="C358" s="23"/>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" s="10"/>
+      <c r="B359" s="10"/>
+      <c r="C359" s="23"/>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360" s="10"/>
+      <c r="B360" s="10"/>
+      <c r="C360" s="23"/>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361" s="10"/>
+      <c r="B361" s="10"/>
+      <c r="C361" s="23"/>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" s="10"/>
+      <c r="B362" s="10"/>
+      <c r="C362" s="23"/>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363" s="10"/>
+      <c r="B363" s="10"/>
+      <c r="C363" s="23"/>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364" s="10"/>
+      <c r="B364" s="10"/>
+      <c r="C364" s="23"/>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365" s="10"/>
+      <c r="B365" s="10"/>
+      <c r="C365" s="23"/>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A366" s="10"/>
+      <c r="B366" s="10"/>
+      <c r="C366" s="23"/>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A367" s="10"/>
+      <c r="B367" s="10"/>
+      <c r="C367" s="23"/>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368" s="10"/>
+      <c r="B368" s="10"/>
+      <c r="C368" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16899,55 +17812,55 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
+        <v>920</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>921</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>922</v>
       </c>
       <c r="C27" s="22"/>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
+        <v>922</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>923</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>924</v>
       </c>
       <c r="C28" s="22"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
+        <v>924</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>925</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>926</v>
       </c>
       <c r="C29" s="22"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
+        <v>926</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>927</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>928</v>
       </c>
       <c r="C30" s="22"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
+        <v>928</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>929</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>930</v>
       </c>
       <c r="C31" s="22"/>
     </row>
     <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>930</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>931</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>932</v>
       </c>
       <c r="C32" s="22"/>
     </row>
@@ -16984,7 +17897,7 @@
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C39" s="22"/>
     </row>

</xml_diff>

<commit_message>
Add translation to weekends with my grandkids history
</commit_message>
<xml_diff>
--- a/english.xlsx
+++ b/english.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popoves\Desktop\experience\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855D4AE6-55DA-4296-9947-307CB5A4B403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1D9D9A-943F-4CD2-92FC-1734F87C9C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="1054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="1067">
   <si>
     <t>word</t>
   </si>
@@ -3043,9 +3043,6 @@
     <t>my wife takes care of the flowers</t>
   </si>
   <si>
-    <t>моя жена ухаживает за растениями</t>
-  </si>
-  <si>
     <t>I take care of the fruits and vegetables</t>
   </si>
   <si>
@@ -3224,6 +3221,48 @@
   </si>
   <si>
     <t>мы всегда с нетерпением ждем их следующего визита</t>
+  </si>
+  <si>
+    <t>I live with my wife Susan</t>
+  </si>
+  <si>
+    <t>we live in small house</t>
+  </si>
+  <si>
+    <t>we live in small house, but we have a big garden</t>
+  </si>
+  <si>
+    <t>we are both retired sowe have a lot of free time</t>
+  </si>
+  <si>
+    <t>we love spending time in our garden</t>
+  </si>
+  <si>
+    <t>моя жена ухаживает за цветами</t>
+  </si>
+  <si>
+    <t>my wife take care of the flowers</t>
+  </si>
+  <si>
+    <t>I take care of fruits and vegetables</t>
+  </si>
+  <si>
+    <t>I teach them how plant and grow vegetables</t>
+  </si>
+  <si>
+    <t>in the evening after dinner</t>
+  </si>
+  <si>
+    <t>we are little sad</t>
+  </si>
+  <si>
+    <t>we are little sad, when it is time for the kids to go home</t>
+  </si>
+  <si>
+    <t>but we are happy to know</t>
+  </si>
+  <si>
+    <t>we always look forvard</t>
   </si>
 </sst>
 </file>
@@ -13958,8 +13997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B299" sqref="B299"/>
+    <sheetView tabSelected="1" topLeftCell="A280" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C299" sqref="C299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16791,7 +16830,9 @@
       <c r="B258" s="10" t="s">
         <v>973</v>
       </c>
-      <c r="C258" s="23"/>
+      <c r="C258" s="8" t="s">
+        <v>972</v>
+      </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="10" t="s">
@@ -16800,7 +16841,9 @@
       <c r="B259" s="10" t="s">
         <v>975</v>
       </c>
-      <c r="C259" s="23"/>
+      <c r="C259" s="8" t="s">
+        <v>974</v>
+      </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="10" t="s">
@@ -16809,7 +16852,9 @@
       <c r="B260" s="10" t="s">
         <v>977</v>
       </c>
-      <c r="C260" s="23"/>
+      <c r="C260" s="8" t="s">
+        <v>1053</v>
+      </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="12" t="s">
@@ -16818,7 +16863,9 @@
       <c r="B261" s="12" t="s">
         <v>981</v>
       </c>
-      <c r="C261" s="23"/>
+      <c r="C261" s="24" t="s">
+        <v>1054</v>
+      </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="12" t="s">
@@ -16827,7 +16874,9 @@
       <c r="B262" s="12" t="s">
         <v>982</v>
       </c>
-      <c r="C262" s="23"/>
+      <c r="C262" s="25" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="10" t="s">
@@ -16836,7 +16885,9 @@
       <c r="B263" s="10" t="s">
         <v>983</v>
       </c>
-      <c r="C263" s="23"/>
+      <c r="C263" s="26" t="s">
+        <v>1055</v>
+      </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="12" t="s">
@@ -16845,7 +16896,9 @@
       <c r="B264" s="12" t="s">
         <v>987</v>
       </c>
-      <c r="C264" s="23"/>
+      <c r="C264" s="24" t="s">
+        <v>984</v>
+      </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
@@ -16854,7 +16907,9 @@
       <c r="B265" s="12" t="s">
         <v>988</v>
       </c>
-      <c r="C265" s="23"/>
+      <c r="C265" s="25" t="s">
+        <v>985</v>
+      </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="10" t="s">
@@ -16863,7 +16918,9 @@
       <c r="B266" s="10" t="s">
         <v>989</v>
       </c>
-      <c r="C266" s="23"/>
+      <c r="C266" s="26" t="s">
+        <v>1056</v>
+      </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="10" t="s">
@@ -16872,286 +16929,350 @@
       <c r="B267" s="10" t="s">
         <v>991</v>
       </c>
-      <c r="C267" s="23"/>
+      <c r="C267" s="8" t="s">
+        <v>1057</v>
+      </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="10" t="s">
         <v>992</v>
       </c>
       <c r="B268" s="10" t="s">
-        <v>993</v>
-      </c>
-      <c r="C268" s="23"/>
+        <v>1058</v>
+      </c>
+      <c r="C268" s="8" t="s">
+        <v>1059</v>
+      </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="10" t="s">
+        <v>993</v>
+      </c>
+      <c r="B269" s="10" t="s">
         <v>994</v>
       </c>
-      <c r="B269" s="10" t="s">
-        <v>995</v>
-      </c>
-      <c r="C269" s="23"/>
+      <c r="C269" s="8" t="s">
+        <v>1060</v>
+      </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="12" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B270" s="12" t="s">
-        <v>999</v>
-      </c>
-      <c r="C270" s="23"/>
+        <v>998</v>
+      </c>
+      <c r="C270" s="24" t="s">
+        <v>995</v>
+      </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B271" s="12" t="s">
-        <v>1000</v>
-      </c>
-      <c r="C271" s="23"/>
+        <v>999</v>
+      </c>
+      <c r="C271" s="25" t="s">
+        <v>996</v>
+      </c>
     </row>
     <row r="272" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="10" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B272" s="10" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C272" s="23"/>
+        <v>1000</v>
+      </c>
+      <c r="C272" s="19" t="s">
+        <v>997</v>
+      </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B273" s="10" t="s">
         <v>1002</v>
       </c>
-      <c r="B273" s="10" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C273" s="23"/>
+      <c r="C273" s="8" t="s">
+        <v>1001</v>
+      </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="10" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B274" s="10" t="s">
         <v>1004</v>
       </c>
-      <c r="B274" s="10" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C274" s="23"/>
+      <c r="C274" s="8" t="s">
+        <v>1003</v>
+      </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="10" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B275" s="10" t="s">
         <v>1006</v>
       </c>
-      <c r="B275" s="10" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C275" s="23"/>
+      <c r="C275" s="8" t="s">
+        <v>1005</v>
+      </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="10" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B276" s="10" t="s">
         <v>1008</v>
       </c>
-      <c r="B276" s="10" t="s">
-        <v>1009</v>
-      </c>
-      <c r="C276" s="23"/>
+      <c r="C276" s="8" t="s">
+        <v>1061</v>
+      </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="10" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B277" s="10" t="s">
         <v>1010</v>
       </c>
-      <c r="B277" s="10" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C277" s="23"/>
+      <c r="C277" s="8" t="s">
+        <v>1009</v>
+      </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="10" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B278" s="10" t="s">
         <v>1012</v>
       </c>
-      <c r="B278" s="10" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C278" s="23"/>
+      <c r="C278" s="8" t="s">
+        <v>1011</v>
+      </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="12" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B279" s="12" t="s">
-        <v>1017</v>
-      </c>
-      <c r="C279" s="23"/>
+        <v>1016</v>
+      </c>
+      <c r="C279" s="24" t="s">
+        <v>1062</v>
+      </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="12" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B280" s="12" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C280" s="23"/>
+        <v>1017</v>
+      </c>
+      <c r="C280" s="25" t="s">
+        <v>1014</v>
+      </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="10" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B281" s="10" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C281" s="23"/>
+        <v>1018</v>
+      </c>
+      <c r="C281" s="26" t="s">
+        <v>1015</v>
+      </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="10" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B282" s="10" t="s">
         <v>1020</v>
       </c>
-      <c r="B282" s="10" t="s">
-        <v>1021</v>
-      </c>
-      <c r="C282" s="23"/>
+      <c r="C282" s="8" t="s">
+        <v>1019</v>
+      </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="10" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B283" s="10" t="s">
         <v>1022</v>
       </c>
-      <c r="B283" s="10" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C283" s="23"/>
+      <c r="C283" s="8" t="s">
+        <v>1021</v>
+      </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="10" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B284" s="10" t="s">
         <v>1024</v>
       </c>
-      <c r="B284" s="10" t="s">
-        <v>1025</v>
-      </c>
-      <c r="C284" s="23"/>
+      <c r="C284" s="8" t="s">
+        <v>1023</v>
+      </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="10" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B285" s="10" t="s">
         <v>1026</v>
       </c>
-      <c r="B285" s="10" t="s">
-        <v>1027</v>
-      </c>
-      <c r="C285" s="23"/>
+      <c r="C285" s="8" t="s">
+        <v>1025</v>
+      </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="10" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B286" s="10" t="s">
         <v>1028</v>
       </c>
-      <c r="B286" s="10" t="s">
-        <v>1029</v>
-      </c>
-      <c r="C286" s="23"/>
+      <c r="C286" s="8" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="10" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B287" s="10" t="s">
         <v>1030</v>
       </c>
-      <c r="B287" s="10" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C287" s="23"/>
+      <c r="C287" s="8" t="s">
+        <v>1029</v>
+      </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="10" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B288" s="10" t="s">
-        <v>1035</v>
-      </c>
-      <c r="C288" s="23"/>
+        <v>1034</v>
+      </c>
+      <c r="C288" s="8" t="s">
+        <v>1031</v>
+      </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B289" s="12" t="s">
         <v>1033</v>
       </c>
-      <c r="B289" s="12" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C289" s="23"/>
+      <c r="C289" s="24" t="s">
+        <v>1063</v>
+      </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="12" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B290" s="12" t="s">
         <v>1036</v>
       </c>
-      <c r="B290" s="12" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C290" s="23"/>
+      <c r="C290" s="25" t="s">
+        <v>1035</v>
+      </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="10" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B291" s="10" t="s">
         <v>1038</v>
       </c>
-      <c r="B291" s="10" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C291" s="23"/>
+      <c r="C291" s="26" t="s">
+        <v>1064</v>
+      </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="10" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B292" s="10" t="s">
         <v>1040</v>
       </c>
-      <c r="B292" s="10" t="s">
-        <v>1041</v>
-      </c>
-      <c r="C292" s="23"/>
+      <c r="C292" s="8" t="s">
+        <v>1039</v>
+      </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B293" s="12" t="s">
         <v>1042</v>
       </c>
-      <c r="B293" s="12" t="s">
-        <v>1043</v>
-      </c>
-      <c r="C293" s="23"/>
+      <c r="C293" s="24" t="s">
+        <v>1065</v>
+      </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="12" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B294" s="12" t="s">
         <v>1044</v>
       </c>
-      <c r="B294" s="12" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C294" s="23"/>
+      <c r="C294" s="25" t="s">
+        <v>1043</v>
+      </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="10" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B295" s="10" t="s">
         <v>1046</v>
       </c>
-      <c r="B295" s="10" t="s">
-        <v>1047</v>
-      </c>
-      <c r="C295" s="23"/>
+      <c r="C295" s="26" t="s">
+        <v>1045</v>
+      </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="10" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B296" s="10" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C296" s="23"/>
+        <v>1050</v>
+      </c>
+      <c r="C296" s="8" t="s">
+        <v>1066</v>
+      </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="10" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B297" s="10" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C297" s="23"/>
+        <v>1051</v>
+      </c>
+      <c r="C297" s="8" t="s">
+        <v>1048</v>
+      </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="10" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B298" s="10" t="s">
-        <v>1053</v>
-      </c>
-      <c r="C298" s="23"/>
+        <v>1052</v>
+      </c>
+      <c r="C298" s="8" t="s">
+        <v>1049</v>
+      </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="10"/>

</xml_diff>